<commit_message>
Start working on 117
</commit_message>
<xml_diff>
--- a/CH-117 Add Index Column.xlsx
+++ b/CH-117 Add Index Column.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBEFDEA2-9DF7-4275-805E-3A4B6CD6A666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC7DD17-6EB3-42B9-B4BF-57CD0378D810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
   <si>
     <t>Question Table</t>
   </si>
@@ -69,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +141,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Sorts Mill Goudy"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Corbel"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -264,10 +294,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -302,8 +333,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -696,7 +734,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="14" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="3"/>
@@ -4024,8 +4062,3413 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{57FE314C-9901-4400-8ACA-E685D11B99D1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37567A5-3451-4387-BA94-B2399B6069E6}">
+  <dimension ref="A1:Z1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" customWidth="1"/>
+    <col min="5" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="26" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="22.5" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9">
+        <v>100</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10">
+        <v>100</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10">
+        <v>45</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10">
+        <v>88</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="10">
+        <v>49</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" ht="14.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="10">
+        <v>43</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10">
+        <v>76</v>
+      </c>
+      <c r="G8" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9">
+        <v>84</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="10">
+        <v>84</v>
+      </c>
+      <c r="G9" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="10">
+        <v>40</v>
+      </c>
+      <c r="G10" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10">
+        <v>69</v>
+      </c>
+      <c r="G11" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="10">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="10">
+        <v>22</v>
+      </c>
+      <c r="G13" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.4">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.4">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.4" customHeight="1">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="14.4">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A18" s="4"/>
+      <c r="B18" s="15" cm="1">
+        <f t="array" ref="B18:B28">_xlfn.MAP(B3:B13,_xlfn.LAMBDA(_xlpm.x,COUNTIF(B3:_xlpm.x,_xlpm.x)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A19" s="4"/>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A22" s="4"/>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="B25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A26" s="4"/>
+      <c r="B26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A27" s="4"/>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.4" customHeight="1">
+      <c r="A28" s="4"/>
+      <c r="B28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A36" s="4"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A91" s="4"/>
+    </row>
+    <row r="92" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A92" s="4"/>
+    </row>
+    <row r="93" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A94" s="4"/>
+    </row>
+    <row r="95" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A96" s="4"/>
+    </row>
+    <row r="97" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A99" s="4"/>
+    </row>
+    <row r="100" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A101" s="4"/>
+    </row>
+    <row r="102" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A102" s="4"/>
+    </row>
+    <row r="103" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A103" s="4"/>
+    </row>
+    <row r="104" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A104" s="4"/>
+    </row>
+    <row r="105" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A105" s="4"/>
+    </row>
+    <row r="106" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A106" s="4"/>
+    </row>
+    <row r="107" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A107" s="4"/>
+    </row>
+    <row r="108" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A108" s="4"/>
+    </row>
+    <row r="109" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A109" s="4"/>
+    </row>
+    <row r="110" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A110" s="4"/>
+    </row>
+    <row r="111" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A111" s="4"/>
+    </row>
+    <row r="112" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A112" s="4"/>
+    </row>
+    <row r="113" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A114" s="4"/>
+    </row>
+    <row r="115" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A116" s="4"/>
+    </row>
+    <row r="117" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A118" s="4"/>
+    </row>
+    <row r="119" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A120" s="4"/>
+    </row>
+    <row r="121" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A121" s="4"/>
+    </row>
+    <row r="122" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A122" s="4"/>
+    </row>
+    <row r="123" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A123" s="4"/>
+    </row>
+    <row r="124" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A124" s="4"/>
+    </row>
+    <row r="125" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A125" s="4"/>
+    </row>
+    <row r="126" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A126" s="4"/>
+    </row>
+    <row r="127" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A127" s="4"/>
+    </row>
+    <row r="128" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A128" s="4"/>
+    </row>
+    <row r="129" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A129" s="4"/>
+    </row>
+    <row r="130" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A130" s="4"/>
+    </row>
+    <row r="131" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A132" s="4"/>
+    </row>
+    <row r="133" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A133" s="4"/>
+    </row>
+    <row r="134" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A134" s="4"/>
+    </row>
+    <row r="135" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A135" s="4"/>
+    </row>
+    <row r="136" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A136" s="4"/>
+    </row>
+    <row r="137" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A137" s="4"/>
+    </row>
+    <row r="138" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A138" s="4"/>
+    </row>
+    <row r="139" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A139" s="4"/>
+    </row>
+    <row r="140" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A140" s="4"/>
+    </row>
+    <row r="141" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A141" s="4"/>
+    </row>
+    <row r="142" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A142" s="4"/>
+    </row>
+    <row r="143" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A143" s="4"/>
+    </row>
+    <row r="144" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A144" s="4"/>
+    </row>
+    <row r="145" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A145" s="4"/>
+    </row>
+    <row r="146" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A146" s="4"/>
+    </row>
+    <row r="147" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A147" s="4"/>
+    </row>
+    <row r="148" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A148" s="4"/>
+    </row>
+    <row r="149" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A149" s="4"/>
+    </row>
+    <row r="150" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A150" s="4"/>
+    </row>
+    <row r="151" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A151" s="4"/>
+    </row>
+    <row r="152" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A152" s="4"/>
+    </row>
+    <row r="153" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A153" s="4"/>
+    </row>
+    <row r="154" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A154" s="4"/>
+    </row>
+    <row r="155" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A155" s="4"/>
+    </row>
+    <row r="156" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A156" s="4"/>
+    </row>
+    <row r="157" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A157" s="4"/>
+    </row>
+    <row r="158" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A158" s="4"/>
+    </row>
+    <row r="159" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A159" s="4"/>
+    </row>
+    <row r="160" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A160" s="4"/>
+    </row>
+    <row r="161" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A161" s="4"/>
+    </row>
+    <row r="162" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A162" s="4"/>
+    </row>
+    <row r="163" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A163" s="4"/>
+    </row>
+    <row r="164" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A164" s="4"/>
+    </row>
+    <row r="165" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A165" s="4"/>
+    </row>
+    <row r="166" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A166" s="4"/>
+    </row>
+    <row r="167" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A167" s="4"/>
+    </row>
+    <row r="168" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A168" s="4"/>
+    </row>
+    <row r="169" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A169" s="4"/>
+    </row>
+    <row r="170" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A170" s="4"/>
+    </row>
+    <row r="171" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A171" s="4"/>
+    </row>
+    <row r="172" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A172" s="4"/>
+    </row>
+    <row r="173" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A173" s="4"/>
+    </row>
+    <row r="174" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A174" s="4"/>
+    </row>
+    <row r="175" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A175" s="4"/>
+    </row>
+    <row r="176" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A176" s="4"/>
+    </row>
+    <row r="177" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A177" s="4"/>
+    </row>
+    <row r="178" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A178" s="4"/>
+    </row>
+    <row r="179" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A179" s="4"/>
+    </row>
+    <row r="180" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A180" s="4"/>
+    </row>
+    <row r="181" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A181" s="4"/>
+    </row>
+    <row r="182" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A182" s="4"/>
+    </row>
+    <row r="183" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A183" s="4"/>
+    </row>
+    <row r="184" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A184" s="4"/>
+    </row>
+    <row r="185" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A185" s="4"/>
+    </row>
+    <row r="186" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A186" s="4"/>
+    </row>
+    <row r="187" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A187" s="4"/>
+    </row>
+    <row r="188" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A188" s="4"/>
+    </row>
+    <row r="189" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A189" s="4"/>
+    </row>
+    <row r="190" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A190" s="4"/>
+    </row>
+    <row r="191" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A191" s="4"/>
+    </row>
+    <row r="192" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A192" s="4"/>
+    </row>
+    <row r="193" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A193" s="4"/>
+    </row>
+    <row r="194" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A194" s="4"/>
+    </row>
+    <row r="195" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A195" s="4"/>
+    </row>
+    <row r="196" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A196" s="4"/>
+    </row>
+    <row r="197" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A197" s="4"/>
+    </row>
+    <row r="198" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A198" s="4"/>
+    </row>
+    <row r="199" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A199" s="4"/>
+    </row>
+    <row r="200" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A200" s="4"/>
+    </row>
+    <row r="201" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A201" s="4"/>
+    </row>
+    <row r="202" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A202" s="4"/>
+    </row>
+    <row r="203" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A203" s="4"/>
+    </row>
+    <row r="204" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A204" s="4"/>
+    </row>
+    <row r="205" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A205" s="4"/>
+    </row>
+    <row r="206" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A206" s="4"/>
+    </row>
+    <row r="207" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A207" s="4"/>
+    </row>
+    <row r="208" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A208" s="4"/>
+    </row>
+    <row r="209" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A209" s="4"/>
+    </row>
+    <row r="210" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A210" s="4"/>
+    </row>
+    <row r="211" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A211" s="4"/>
+    </row>
+    <row r="212" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A212" s="4"/>
+    </row>
+    <row r="213" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A213" s="4"/>
+    </row>
+    <row r="214" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A214" s="4"/>
+    </row>
+    <row r="215" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A215" s="4"/>
+    </row>
+    <row r="216" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A216" s="4"/>
+    </row>
+    <row r="217" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A217" s="4"/>
+    </row>
+    <row r="218" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A218" s="4"/>
+    </row>
+    <row r="219" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A219" s="4"/>
+    </row>
+    <row r="220" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A220" s="4"/>
+    </row>
+    <row r="221" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A221" s="4"/>
+    </row>
+    <row r="222" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A222" s="4"/>
+    </row>
+    <row r="223" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A223" s="4"/>
+    </row>
+    <row r="224" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A224" s="4"/>
+    </row>
+    <row r="225" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A225" s="4"/>
+    </row>
+    <row r="226" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A226" s="4"/>
+    </row>
+    <row r="227" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A227" s="4"/>
+    </row>
+    <row r="228" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A228" s="4"/>
+    </row>
+    <row r="229" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A229" s="4"/>
+    </row>
+    <row r="230" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A230" s="4"/>
+    </row>
+    <row r="231" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A231" s="4"/>
+    </row>
+    <row r="232" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A232" s="4"/>
+    </row>
+    <row r="233" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A233" s="4"/>
+    </row>
+    <row r="234" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A234" s="4"/>
+    </row>
+    <row r="235" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A235" s="4"/>
+    </row>
+    <row r="236" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A236" s="4"/>
+    </row>
+    <row r="237" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A237" s="4"/>
+    </row>
+    <row r="238" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A238" s="4"/>
+    </row>
+    <row r="239" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A239" s="4"/>
+    </row>
+    <row r="240" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A240" s="4"/>
+    </row>
+    <row r="241" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A241" s="4"/>
+    </row>
+    <row r="242" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A242" s="4"/>
+    </row>
+    <row r="243" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A243" s="4"/>
+    </row>
+    <row r="244" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A244" s="4"/>
+    </row>
+    <row r="245" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A245" s="4"/>
+    </row>
+    <row r="246" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A246" s="4"/>
+    </row>
+    <row r="247" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A247" s="4"/>
+    </row>
+    <row r="248" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A248" s="4"/>
+    </row>
+    <row r="249" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A249" s="4"/>
+    </row>
+    <row r="250" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A250" s="4"/>
+    </row>
+    <row r="251" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A251" s="4"/>
+    </row>
+    <row r="252" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A252" s="4"/>
+    </row>
+    <row r="253" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A253" s="4"/>
+    </row>
+    <row r="254" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A254" s="4"/>
+    </row>
+    <row r="255" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A255" s="4"/>
+    </row>
+    <row r="256" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A256" s="4"/>
+    </row>
+    <row r="257" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A257" s="4"/>
+    </row>
+    <row r="258" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A258" s="4"/>
+    </row>
+    <row r="259" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A259" s="4"/>
+    </row>
+    <row r="260" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A260" s="4"/>
+    </row>
+    <row r="261" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A261" s="4"/>
+    </row>
+    <row r="262" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A262" s="4"/>
+    </row>
+    <row r="263" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A263" s="4"/>
+    </row>
+    <row r="264" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A264" s="4"/>
+    </row>
+    <row r="265" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A265" s="4"/>
+    </row>
+    <row r="266" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A266" s="4"/>
+    </row>
+    <row r="267" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A267" s="4"/>
+    </row>
+    <row r="268" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A268" s="4"/>
+    </row>
+    <row r="269" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A269" s="4"/>
+    </row>
+    <row r="270" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A270" s="4"/>
+    </row>
+    <row r="271" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A271" s="4"/>
+    </row>
+    <row r="272" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A272" s="4"/>
+    </row>
+    <row r="273" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A273" s="4"/>
+    </row>
+    <row r="274" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A274" s="4"/>
+    </row>
+    <row r="275" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A275" s="4"/>
+    </row>
+    <row r="276" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A276" s="4"/>
+    </row>
+    <row r="277" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A277" s="4"/>
+    </row>
+    <row r="278" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A278" s="4"/>
+    </row>
+    <row r="279" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A279" s="4"/>
+    </row>
+    <row r="280" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A280" s="4"/>
+    </row>
+    <row r="281" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A281" s="4"/>
+    </row>
+    <row r="282" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A282" s="4"/>
+    </row>
+    <row r="283" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A283" s="4"/>
+    </row>
+    <row r="284" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A284" s="4"/>
+    </row>
+    <row r="285" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A285" s="4"/>
+    </row>
+    <row r="286" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A286" s="4"/>
+    </row>
+    <row r="287" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A287" s="4"/>
+    </row>
+    <row r="288" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A288" s="4"/>
+    </row>
+    <row r="289" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A289" s="4"/>
+    </row>
+    <row r="290" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A290" s="4"/>
+    </row>
+    <row r="291" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A291" s="4"/>
+    </row>
+    <row r="292" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A292" s="4"/>
+    </row>
+    <row r="293" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A293" s="4"/>
+    </row>
+    <row r="294" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A294" s="4"/>
+    </row>
+    <row r="295" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A295" s="4"/>
+    </row>
+    <row r="296" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A296" s="4"/>
+    </row>
+    <row r="297" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A297" s="4"/>
+    </row>
+    <row r="298" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A298" s="4"/>
+    </row>
+    <row r="299" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A299" s="4"/>
+    </row>
+    <row r="300" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A300" s="4"/>
+    </row>
+    <row r="301" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A301" s="4"/>
+    </row>
+    <row r="302" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A302" s="4"/>
+    </row>
+    <row r="303" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A303" s="4"/>
+    </row>
+    <row r="304" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A304" s="4"/>
+    </row>
+    <row r="305" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A305" s="4"/>
+    </row>
+    <row r="306" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A306" s="4"/>
+    </row>
+    <row r="307" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A307" s="4"/>
+    </row>
+    <row r="308" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A308" s="4"/>
+    </row>
+    <row r="309" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A309" s="4"/>
+    </row>
+    <row r="310" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A310" s="4"/>
+    </row>
+    <row r="311" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A311" s="4"/>
+    </row>
+    <row r="312" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A312" s="4"/>
+    </row>
+    <row r="313" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A313" s="4"/>
+    </row>
+    <row r="314" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A314" s="4"/>
+    </row>
+    <row r="315" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A315" s="4"/>
+    </row>
+    <row r="316" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A316" s="4"/>
+    </row>
+    <row r="317" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A317" s="4"/>
+    </row>
+    <row r="318" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A318" s="4"/>
+    </row>
+    <row r="319" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A319" s="4"/>
+    </row>
+    <row r="320" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A320" s="4"/>
+    </row>
+    <row r="321" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A321" s="4"/>
+    </row>
+    <row r="322" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A322" s="4"/>
+    </row>
+    <row r="323" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A323" s="4"/>
+    </row>
+    <row r="324" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A324" s="4"/>
+    </row>
+    <row r="325" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A325" s="4"/>
+    </row>
+    <row r="326" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A326" s="4"/>
+    </row>
+    <row r="327" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A327" s="4"/>
+    </row>
+    <row r="328" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A328" s="4"/>
+    </row>
+    <row r="329" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A329" s="4"/>
+    </row>
+    <row r="330" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A330" s="4"/>
+    </row>
+    <row r="331" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A331" s="4"/>
+    </row>
+    <row r="332" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A332" s="4"/>
+    </row>
+    <row r="333" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A333" s="4"/>
+    </row>
+    <row r="334" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A334" s="4"/>
+    </row>
+    <row r="335" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A335" s="4"/>
+    </row>
+    <row r="336" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A336" s="4"/>
+    </row>
+    <row r="337" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A337" s="4"/>
+    </row>
+    <row r="338" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A338" s="4"/>
+    </row>
+    <row r="339" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A339" s="4"/>
+    </row>
+    <row r="340" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A340" s="4"/>
+    </row>
+    <row r="341" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A341" s="4"/>
+    </row>
+    <row r="342" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A342" s="4"/>
+    </row>
+    <row r="343" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A343" s="4"/>
+    </row>
+    <row r="344" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A344" s="4"/>
+    </row>
+    <row r="345" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A345" s="4"/>
+    </row>
+    <row r="346" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A346" s="4"/>
+    </row>
+    <row r="347" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A347" s="4"/>
+    </row>
+    <row r="348" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A348" s="4"/>
+    </row>
+    <row r="349" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A349" s="4"/>
+    </row>
+    <row r="350" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A350" s="4"/>
+    </row>
+    <row r="351" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A351" s="4"/>
+    </row>
+    <row r="352" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A352" s="4"/>
+    </row>
+    <row r="353" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A353" s="4"/>
+    </row>
+    <row r="354" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A354" s="4"/>
+    </row>
+    <row r="355" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A355" s="4"/>
+    </row>
+    <row r="356" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A356" s="4"/>
+    </row>
+    <row r="357" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A357" s="4"/>
+    </row>
+    <row r="358" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A358" s="4"/>
+    </row>
+    <row r="359" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A359" s="4"/>
+    </row>
+    <row r="360" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A360" s="4"/>
+    </row>
+    <row r="361" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A361" s="4"/>
+    </row>
+    <row r="362" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A362" s="4"/>
+    </row>
+    <row r="363" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A363" s="4"/>
+    </row>
+    <row r="364" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A364" s="4"/>
+    </row>
+    <row r="365" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A365" s="4"/>
+    </row>
+    <row r="366" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A366" s="4"/>
+    </row>
+    <row r="367" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A367" s="4"/>
+    </row>
+    <row r="368" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A368" s="4"/>
+    </row>
+    <row r="369" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A369" s="4"/>
+    </row>
+    <row r="370" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A370" s="4"/>
+    </row>
+    <row r="371" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A371" s="4"/>
+    </row>
+    <row r="372" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A372" s="4"/>
+    </row>
+    <row r="373" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A373" s="4"/>
+    </row>
+    <row r="374" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A374" s="4"/>
+    </row>
+    <row r="375" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A375" s="4"/>
+    </row>
+    <row r="376" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A376" s="4"/>
+    </row>
+    <row r="377" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A377" s="4"/>
+    </row>
+    <row r="378" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A378" s="4"/>
+    </row>
+    <row r="379" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A379" s="4"/>
+    </row>
+    <row r="380" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A380" s="4"/>
+    </row>
+    <row r="381" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A381" s="4"/>
+    </row>
+    <row r="382" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A382" s="4"/>
+    </row>
+    <row r="383" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A383" s="4"/>
+    </row>
+    <row r="384" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A384" s="4"/>
+    </row>
+    <row r="385" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A385" s="4"/>
+    </row>
+    <row r="386" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A386" s="4"/>
+    </row>
+    <row r="387" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A387" s="4"/>
+    </row>
+    <row r="388" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A388" s="4"/>
+    </row>
+    <row r="389" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A389" s="4"/>
+    </row>
+    <row r="390" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A390" s="4"/>
+    </row>
+    <row r="391" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A391" s="4"/>
+    </row>
+    <row r="392" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A392" s="4"/>
+    </row>
+    <row r="393" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A393" s="4"/>
+    </row>
+    <row r="394" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A394" s="4"/>
+    </row>
+    <row r="395" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A395" s="4"/>
+    </row>
+    <row r="396" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A396" s="4"/>
+    </row>
+    <row r="397" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A397" s="4"/>
+    </row>
+    <row r="398" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A398" s="4"/>
+    </row>
+    <row r="399" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A399" s="4"/>
+    </row>
+    <row r="400" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A400" s="4"/>
+    </row>
+    <row r="401" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A401" s="4"/>
+    </row>
+    <row r="402" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A402" s="4"/>
+    </row>
+    <row r="403" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A403" s="4"/>
+    </row>
+    <row r="404" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A404" s="4"/>
+    </row>
+    <row r="405" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A405" s="4"/>
+    </row>
+    <row r="406" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A406" s="4"/>
+    </row>
+    <row r="407" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A407" s="4"/>
+    </row>
+    <row r="408" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A408" s="4"/>
+    </row>
+    <row r="409" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A409" s="4"/>
+    </row>
+    <row r="410" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A410" s="4"/>
+    </row>
+    <row r="411" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A411" s="4"/>
+    </row>
+    <row r="412" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A412" s="4"/>
+    </row>
+    <row r="413" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A413" s="4"/>
+    </row>
+    <row r="414" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A414" s="4"/>
+    </row>
+    <row r="415" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A415" s="4"/>
+    </row>
+    <row r="416" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A416" s="4"/>
+    </row>
+    <row r="417" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A417" s="4"/>
+    </row>
+    <row r="418" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A418" s="4"/>
+    </row>
+    <row r="419" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A419" s="4"/>
+    </row>
+    <row r="420" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A420" s="4"/>
+    </row>
+    <row r="421" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A421" s="4"/>
+    </row>
+    <row r="422" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A422" s="4"/>
+    </row>
+    <row r="423" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A423" s="4"/>
+    </row>
+    <row r="424" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A424" s="4"/>
+    </row>
+    <row r="425" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A425" s="4"/>
+    </row>
+    <row r="426" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A426" s="4"/>
+    </row>
+    <row r="427" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A427" s="4"/>
+    </row>
+    <row r="428" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A428" s="4"/>
+    </row>
+    <row r="429" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A429" s="4"/>
+    </row>
+    <row r="430" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A430" s="4"/>
+    </row>
+    <row r="431" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A431" s="4"/>
+    </row>
+    <row r="432" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A432" s="4"/>
+    </row>
+    <row r="433" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A433" s="4"/>
+    </row>
+    <row r="434" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A434" s="4"/>
+    </row>
+    <row r="435" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A435" s="4"/>
+    </row>
+    <row r="436" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A436" s="4"/>
+    </row>
+    <row r="437" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A437" s="4"/>
+    </row>
+    <row r="438" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A438" s="4"/>
+    </row>
+    <row r="439" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A439" s="4"/>
+    </row>
+    <row r="440" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A440" s="4"/>
+    </row>
+    <row r="441" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A441" s="4"/>
+    </row>
+    <row r="442" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A442" s="4"/>
+    </row>
+    <row r="443" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A443" s="4"/>
+    </row>
+    <row r="444" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A444" s="4"/>
+    </row>
+    <row r="445" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A445" s="4"/>
+    </row>
+    <row r="446" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A446" s="4"/>
+    </row>
+    <row r="447" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A447" s="4"/>
+    </row>
+    <row r="448" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A448" s="4"/>
+    </row>
+    <row r="449" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A449" s="4"/>
+    </row>
+    <row r="450" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A450" s="4"/>
+    </row>
+    <row r="451" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A451" s="4"/>
+    </row>
+    <row r="452" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A452" s="4"/>
+    </row>
+    <row r="453" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A453" s="4"/>
+    </row>
+    <row r="454" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A454" s="4"/>
+    </row>
+    <row r="455" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A455" s="4"/>
+    </row>
+    <row r="456" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A456" s="4"/>
+    </row>
+    <row r="457" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A457" s="4"/>
+    </row>
+    <row r="458" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A458" s="4"/>
+    </row>
+    <row r="459" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A459" s="4"/>
+    </row>
+    <row r="460" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A460" s="4"/>
+    </row>
+    <row r="461" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A461" s="4"/>
+    </row>
+    <row r="462" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A462" s="4"/>
+    </row>
+    <row r="463" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A463" s="4"/>
+    </row>
+    <row r="464" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A464" s="4"/>
+    </row>
+    <row r="465" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A465" s="4"/>
+    </row>
+    <row r="466" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A466" s="4"/>
+    </row>
+    <row r="467" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A467" s="4"/>
+    </row>
+    <row r="468" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A468" s="4"/>
+    </row>
+    <row r="469" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A469" s="4"/>
+    </row>
+    <row r="470" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A470" s="4"/>
+    </row>
+    <row r="471" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A471" s="4"/>
+    </row>
+    <row r="472" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A472" s="4"/>
+    </row>
+    <row r="473" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A473" s="4"/>
+    </row>
+    <row r="474" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A474" s="4"/>
+    </row>
+    <row r="475" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A475" s="4"/>
+    </row>
+    <row r="476" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A476" s="4"/>
+    </row>
+    <row r="477" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A477" s="4"/>
+    </row>
+    <row r="478" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A478" s="4"/>
+    </row>
+    <row r="479" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A479" s="4"/>
+    </row>
+    <row r="480" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A480" s="4"/>
+    </row>
+    <row r="481" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A481" s="4"/>
+    </row>
+    <row r="482" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A482" s="4"/>
+    </row>
+    <row r="483" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A483" s="4"/>
+    </row>
+    <row r="484" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A484" s="4"/>
+    </row>
+    <row r="485" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A485" s="4"/>
+    </row>
+    <row r="486" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A486" s="4"/>
+    </row>
+    <row r="487" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A487" s="4"/>
+    </row>
+    <row r="488" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A488" s="4"/>
+    </row>
+    <row r="489" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A489" s="4"/>
+    </row>
+    <row r="490" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A490" s="4"/>
+    </row>
+    <row r="491" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A491" s="4"/>
+    </row>
+    <row r="492" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A492" s="4"/>
+    </row>
+    <row r="493" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A493" s="4"/>
+    </row>
+    <row r="494" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A494" s="4"/>
+    </row>
+    <row r="495" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A495" s="4"/>
+    </row>
+    <row r="496" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A496" s="4"/>
+    </row>
+    <row r="497" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A497" s="4"/>
+    </row>
+    <row r="498" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A498" s="4"/>
+    </row>
+    <row r="499" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A499" s="4"/>
+    </row>
+    <row r="500" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A500" s="4"/>
+    </row>
+    <row r="501" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A501" s="4"/>
+    </row>
+    <row r="502" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A502" s="4"/>
+    </row>
+    <row r="503" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A503" s="4"/>
+    </row>
+    <row r="504" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A504" s="4"/>
+    </row>
+    <row r="505" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A505" s="4"/>
+    </row>
+    <row r="506" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A506" s="4"/>
+    </row>
+    <row r="507" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A507" s="4"/>
+    </row>
+    <row r="508" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A508" s="4"/>
+    </row>
+    <row r="509" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A509" s="4"/>
+    </row>
+    <row r="510" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A510" s="4"/>
+    </row>
+    <row r="511" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A511" s="4"/>
+    </row>
+    <row r="512" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A512" s="4"/>
+    </row>
+    <row r="513" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A513" s="4"/>
+    </row>
+    <row r="514" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A514" s="4"/>
+    </row>
+    <row r="515" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A515" s="4"/>
+    </row>
+    <row r="516" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A516" s="4"/>
+    </row>
+    <row r="517" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A517" s="4"/>
+    </row>
+    <row r="518" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A518" s="4"/>
+    </row>
+    <row r="519" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A519" s="4"/>
+    </row>
+    <row r="520" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A520" s="4"/>
+    </row>
+    <row r="521" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A521" s="4"/>
+    </row>
+    <row r="522" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A522" s="4"/>
+    </row>
+    <row r="523" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A523" s="4"/>
+    </row>
+    <row r="524" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A524" s="4"/>
+    </row>
+    <row r="525" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A525" s="4"/>
+    </row>
+    <row r="526" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A526" s="4"/>
+    </row>
+    <row r="527" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A527" s="4"/>
+    </row>
+    <row r="528" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A528" s="4"/>
+    </row>
+    <row r="529" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A529" s="4"/>
+    </row>
+    <row r="530" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A530" s="4"/>
+    </row>
+    <row r="531" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A531" s="4"/>
+    </row>
+    <row r="532" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A532" s="4"/>
+    </row>
+    <row r="533" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A533" s="4"/>
+    </row>
+    <row r="534" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A534" s="4"/>
+    </row>
+    <row r="535" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A535" s="4"/>
+    </row>
+    <row r="536" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A536" s="4"/>
+    </row>
+    <row r="537" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A537" s="4"/>
+    </row>
+    <row r="538" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A538" s="4"/>
+    </row>
+    <row r="539" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A539" s="4"/>
+    </row>
+    <row r="540" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A540" s="4"/>
+    </row>
+    <row r="541" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A541" s="4"/>
+    </row>
+    <row r="542" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A542" s="4"/>
+    </row>
+    <row r="543" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A543" s="4"/>
+    </row>
+    <row r="544" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A544" s="4"/>
+    </row>
+    <row r="545" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A545" s="4"/>
+    </row>
+    <row r="546" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A546" s="4"/>
+    </row>
+    <row r="547" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A547" s="4"/>
+    </row>
+    <row r="548" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A548" s="4"/>
+    </row>
+    <row r="549" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A549" s="4"/>
+    </row>
+    <row r="550" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A550" s="4"/>
+    </row>
+    <row r="551" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A551" s="4"/>
+    </row>
+    <row r="552" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A552" s="4"/>
+    </row>
+    <row r="553" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A553" s="4"/>
+    </row>
+    <row r="554" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A554" s="4"/>
+    </row>
+    <row r="555" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A555" s="4"/>
+    </row>
+    <row r="556" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A556" s="4"/>
+    </row>
+    <row r="557" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A557" s="4"/>
+    </row>
+    <row r="558" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A558" s="4"/>
+    </row>
+    <row r="559" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A559" s="4"/>
+    </row>
+    <row r="560" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A560" s="4"/>
+    </row>
+    <row r="561" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A561" s="4"/>
+    </row>
+    <row r="562" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A562" s="4"/>
+    </row>
+    <row r="563" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A563" s="4"/>
+    </row>
+    <row r="564" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A564" s="4"/>
+    </row>
+    <row r="565" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A565" s="4"/>
+    </row>
+    <row r="566" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A566" s="4"/>
+    </row>
+    <row r="567" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A567" s="4"/>
+    </row>
+    <row r="568" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A568" s="4"/>
+    </row>
+    <row r="569" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A569" s="4"/>
+    </row>
+    <row r="570" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A570" s="4"/>
+    </row>
+    <row r="571" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A571" s="4"/>
+    </row>
+    <row r="572" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A572" s="4"/>
+    </row>
+    <row r="573" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A573" s="4"/>
+    </row>
+    <row r="574" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A574" s="4"/>
+    </row>
+    <row r="575" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A575" s="4"/>
+    </row>
+    <row r="576" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A576" s="4"/>
+    </row>
+    <row r="577" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A577" s="4"/>
+    </row>
+    <row r="578" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A578" s="4"/>
+    </row>
+    <row r="579" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A579" s="4"/>
+    </row>
+    <row r="580" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A580" s="4"/>
+    </row>
+    <row r="581" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A581" s="4"/>
+    </row>
+    <row r="582" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A582" s="4"/>
+    </row>
+    <row r="583" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A583" s="4"/>
+    </row>
+    <row r="584" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A584" s="4"/>
+    </row>
+    <row r="585" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A585" s="4"/>
+    </row>
+    <row r="586" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A586" s="4"/>
+    </row>
+    <row r="587" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A587" s="4"/>
+    </row>
+    <row r="588" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A588" s="4"/>
+    </row>
+    <row r="589" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A589" s="4"/>
+    </row>
+    <row r="590" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A590" s="4"/>
+    </row>
+    <row r="591" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A591" s="4"/>
+    </row>
+    <row r="592" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A592" s="4"/>
+    </row>
+    <row r="593" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A593" s="4"/>
+    </row>
+    <row r="594" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A594" s="4"/>
+    </row>
+    <row r="595" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A595" s="4"/>
+    </row>
+    <row r="596" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A596" s="4"/>
+    </row>
+    <row r="597" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A597" s="4"/>
+    </row>
+    <row r="598" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A598" s="4"/>
+    </row>
+    <row r="599" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A599" s="4"/>
+    </row>
+    <row r="600" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A600" s="4"/>
+    </row>
+    <row r="601" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A601" s="4"/>
+    </row>
+    <row r="602" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A602" s="4"/>
+    </row>
+    <row r="603" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A603" s="4"/>
+    </row>
+    <row r="604" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A604" s="4"/>
+    </row>
+    <row r="605" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A605" s="4"/>
+    </row>
+    <row r="606" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A606" s="4"/>
+    </row>
+    <row r="607" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A607" s="4"/>
+    </row>
+    <row r="608" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A608" s="4"/>
+    </row>
+    <row r="609" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A609" s="4"/>
+    </row>
+    <row r="610" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A610" s="4"/>
+    </row>
+    <row r="611" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A611" s="4"/>
+    </row>
+    <row r="612" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A612" s="4"/>
+    </row>
+    <row r="613" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A613" s="4"/>
+    </row>
+    <row r="614" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A614" s="4"/>
+    </row>
+    <row r="615" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A615" s="4"/>
+    </row>
+    <row r="616" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A616" s="4"/>
+    </row>
+    <row r="617" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A617" s="4"/>
+    </row>
+    <row r="618" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A618" s="4"/>
+    </row>
+    <row r="619" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A619" s="4"/>
+    </row>
+    <row r="620" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A620" s="4"/>
+    </row>
+    <row r="621" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A621" s="4"/>
+    </row>
+    <row r="622" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A622" s="4"/>
+    </row>
+    <row r="623" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A623" s="4"/>
+    </row>
+    <row r="624" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A624" s="4"/>
+    </row>
+    <row r="625" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A625" s="4"/>
+    </row>
+    <row r="626" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A626" s="4"/>
+    </row>
+    <row r="627" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A627" s="4"/>
+    </row>
+    <row r="628" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A628" s="4"/>
+    </row>
+    <row r="629" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A629" s="4"/>
+    </row>
+    <row r="630" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A630" s="4"/>
+    </row>
+    <row r="631" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A631" s="4"/>
+    </row>
+    <row r="632" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A632" s="4"/>
+    </row>
+    <row r="633" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A633" s="4"/>
+    </row>
+    <row r="634" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A634" s="4"/>
+    </row>
+    <row r="635" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A635" s="4"/>
+    </row>
+    <row r="636" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A636" s="4"/>
+    </row>
+    <row r="637" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A637" s="4"/>
+    </row>
+    <row r="638" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A638" s="4"/>
+    </row>
+    <row r="639" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A639" s="4"/>
+    </row>
+    <row r="640" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A640" s="4"/>
+    </row>
+    <row r="641" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A641" s="4"/>
+    </row>
+    <row r="642" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A642" s="4"/>
+    </row>
+    <row r="643" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A643" s="4"/>
+    </row>
+    <row r="644" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A644" s="4"/>
+    </row>
+    <row r="645" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A645" s="4"/>
+    </row>
+    <row r="646" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A646" s="4"/>
+    </row>
+    <row r="647" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A647" s="4"/>
+    </row>
+    <row r="648" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A648" s="4"/>
+    </row>
+    <row r="649" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A649" s="4"/>
+    </row>
+    <row r="650" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A650" s="4"/>
+    </row>
+    <row r="651" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A651" s="4"/>
+    </row>
+    <row r="652" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A652" s="4"/>
+    </row>
+    <row r="653" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A653" s="4"/>
+    </row>
+    <row r="654" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A654" s="4"/>
+    </row>
+    <row r="655" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A655" s="4"/>
+    </row>
+    <row r="656" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A656" s="4"/>
+    </row>
+    <row r="657" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A657" s="4"/>
+    </row>
+    <row r="658" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A658" s="4"/>
+    </row>
+    <row r="659" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A659" s="4"/>
+    </row>
+    <row r="660" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A660" s="4"/>
+    </row>
+    <row r="661" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A661" s="4"/>
+    </row>
+    <row r="662" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A662" s="4"/>
+    </row>
+    <row r="663" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A663" s="4"/>
+    </row>
+    <row r="664" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A664" s="4"/>
+    </row>
+    <row r="665" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A665" s="4"/>
+    </row>
+    <row r="666" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A666" s="4"/>
+    </row>
+    <row r="667" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A667" s="4"/>
+    </row>
+    <row r="668" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A668" s="4"/>
+    </row>
+    <row r="669" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A669" s="4"/>
+    </row>
+    <row r="670" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A670" s="4"/>
+    </row>
+    <row r="671" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A671" s="4"/>
+    </row>
+    <row r="672" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A672" s="4"/>
+    </row>
+    <row r="673" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A673" s="4"/>
+    </row>
+    <row r="674" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A674" s="4"/>
+    </row>
+    <row r="675" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A675" s="4"/>
+    </row>
+    <row r="676" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A676" s="4"/>
+    </row>
+    <row r="677" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A677" s="4"/>
+    </row>
+    <row r="678" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A678" s="4"/>
+    </row>
+    <row r="679" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A679" s="4"/>
+    </row>
+    <row r="680" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A680" s="4"/>
+    </row>
+    <row r="681" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A681" s="4"/>
+    </row>
+    <row r="682" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A682" s="4"/>
+    </row>
+    <row r="683" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A683" s="4"/>
+    </row>
+    <row r="684" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A684" s="4"/>
+    </row>
+    <row r="685" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A685" s="4"/>
+    </row>
+    <row r="686" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A686" s="4"/>
+    </row>
+    <row r="687" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A687" s="4"/>
+    </row>
+    <row r="688" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A688" s="4"/>
+    </row>
+    <row r="689" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A689" s="4"/>
+    </row>
+    <row r="690" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A690" s="4"/>
+    </row>
+    <row r="691" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A691" s="4"/>
+    </row>
+    <row r="692" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A692" s="4"/>
+    </row>
+    <row r="693" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A693" s="4"/>
+    </row>
+    <row r="694" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A694" s="4"/>
+    </row>
+    <row r="695" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A695" s="4"/>
+    </row>
+    <row r="696" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A696" s="4"/>
+    </row>
+    <row r="697" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A697" s="4"/>
+    </row>
+    <row r="698" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A698" s="4"/>
+    </row>
+    <row r="699" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A699" s="4"/>
+    </row>
+    <row r="700" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A700" s="4"/>
+    </row>
+    <row r="701" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A701" s="4"/>
+    </row>
+    <row r="702" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A702" s="4"/>
+    </row>
+    <row r="703" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A703" s="4"/>
+    </row>
+    <row r="704" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A704" s="4"/>
+    </row>
+    <row r="705" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A705" s="4"/>
+    </row>
+    <row r="706" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A706" s="4"/>
+    </row>
+    <row r="707" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A707" s="4"/>
+    </row>
+    <row r="708" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A708" s="4"/>
+    </row>
+    <row r="709" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A709" s="4"/>
+    </row>
+    <row r="710" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A710" s="4"/>
+    </row>
+    <row r="711" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A711" s="4"/>
+    </row>
+    <row r="712" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A712" s="4"/>
+    </row>
+    <row r="713" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A713" s="4"/>
+    </row>
+    <row r="714" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A714" s="4"/>
+    </row>
+    <row r="715" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A715" s="4"/>
+    </row>
+    <row r="716" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A716" s="4"/>
+    </row>
+    <row r="717" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A717" s="4"/>
+    </row>
+    <row r="718" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A718" s="4"/>
+    </row>
+    <row r="719" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A719" s="4"/>
+    </row>
+    <row r="720" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A720" s="4"/>
+    </row>
+    <row r="721" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A721" s="4"/>
+    </row>
+    <row r="722" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A722" s="4"/>
+    </row>
+    <row r="723" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A723" s="4"/>
+    </row>
+    <row r="724" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A724" s="4"/>
+    </row>
+    <row r="725" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A725" s="4"/>
+    </row>
+    <row r="726" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A726" s="4"/>
+    </row>
+    <row r="727" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A727" s="4"/>
+    </row>
+    <row r="728" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A728" s="4"/>
+    </row>
+    <row r="729" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A729" s="4"/>
+    </row>
+    <row r="730" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A730" s="4"/>
+    </row>
+    <row r="731" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A731" s="4"/>
+    </row>
+    <row r="732" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A732" s="4"/>
+    </row>
+    <row r="733" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A733" s="4"/>
+    </row>
+    <row r="734" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A734" s="4"/>
+    </row>
+    <row r="735" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A735" s="4"/>
+    </row>
+    <row r="736" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A736" s="4"/>
+    </row>
+    <row r="737" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A737" s="4"/>
+    </row>
+    <row r="738" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A738" s="4"/>
+    </row>
+    <row r="739" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A739" s="4"/>
+    </row>
+    <row r="740" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A740" s="4"/>
+    </row>
+    <row r="741" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A741" s="4"/>
+    </row>
+    <row r="742" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A742" s="4"/>
+    </row>
+    <row r="743" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A743" s="4"/>
+    </row>
+    <row r="744" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A744" s="4"/>
+    </row>
+    <row r="745" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A745" s="4"/>
+    </row>
+    <row r="746" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A746" s="4"/>
+    </row>
+    <row r="747" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A747" s="4"/>
+    </row>
+    <row r="748" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A748" s="4"/>
+    </row>
+    <row r="749" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A749" s="4"/>
+    </row>
+    <row r="750" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A750" s="4"/>
+    </row>
+    <row r="751" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A751" s="4"/>
+    </row>
+    <row r="752" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A752" s="4"/>
+    </row>
+    <row r="753" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A753" s="4"/>
+    </row>
+    <row r="754" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A754" s="4"/>
+    </row>
+    <row r="755" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A755" s="4"/>
+    </row>
+    <row r="756" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A756" s="4"/>
+    </row>
+    <row r="757" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A757" s="4"/>
+    </row>
+    <row r="758" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A758" s="4"/>
+    </row>
+    <row r="759" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A759" s="4"/>
+    </row>
+    <row r="760" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A760" s="4"/>
+    </row>
+    <row r="761" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A761" s="4"/>
+    </row>
+    <row r="762" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A762" s="4"/>
+    </row>
+    <row r="763" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A763" s="4"/>
+    </row>
+    <row r="764" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A764" s="4"/>
+    </row>
+    <row r="765" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A765" s="4"/>
+    </row>
+    <row r="766" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A766" s="4"/>
+    </row>
+    <row r="767" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A767" s="4"/>
+    </row>
+    <row r="768" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A768" s="4"/>
+    </row>
+    <row r="769" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A769" s="4"/>
+    </row>
+    <row r="770" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A770" s="4"/>
+    </row>
+    <row r="771" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A771" s="4"/>
+    </row>
+    <row r="772" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A772" s="4"/>
+    </row>
+    <row r="773" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A773" s="4"/>
+    </row>
+    <row r="774" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A774" s="4"/>
+    </row>
+    <row r="775" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A775" s="4"/>
+    </row>
+    <row r="776" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A776" s="4"/>
+    </row>
+    <row r="777" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A777" s="4"/>
+    </row>
+    <row r="778" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A778" s="4"/>
+    </row>
+    <row r="779" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A779" s="4"/>
+    </row>
+    <row r="780" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A780" s="4"/>
+    </row>
+    <row r="781" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A781" s="4"/>
+    </row>
+    <row r="782" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A782" s="4"/>
+    </row>
+    <row r="783" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A783" s="4"/>
+    </row>
+    <row r="784" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A784" s="4"/>
+    </row>
+    <row r="785" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A785" s="4"/>
+    </row>
+    <row r="786" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A786" s="4"/>
+    </row>
+    <row r="787" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A787" s="4"/>
+    </row>
+    <row r="788" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A788" s="4"/>
+    </row>
+    <row r="789" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A789" s="4"/>
+    </row>
+    <row r="790" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A790" s="4"/>
+    </row>
+    <row r="791" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A791" s="4"/>
+    </row>
+    <row r="792" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A792" s="4"/>
+    </row>
+    <row r="793" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A793" s="4"/>
+    </row>
+    <row r="794" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A794" s="4"/>
+    </row>
+    <row r="795" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A795" s="4"/>
+    </row>
+    <row r="796" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A796" s="4"/>
+    </row>
+    <row r="797" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A797" s="4"/>
+    </row>
+    <row r="798" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A798" s="4"/>
+    </row>
+    <row r="799" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A799" s="4"/>
+    </row>
+    <row r="800" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A800" s="4"/>
+    </row>
+    <row r="801" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A801" s="4"/>
+    </row>
+    <row r="802" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A802" s="4"/>
+    </row>
+    <row r="803" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A803" s="4"/>
+    </row>
+    <row r="804" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A804" s="4"/>
+    </row>
+    <row r="805" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A805" s="4"/>
+    </row>
+    <row r="806" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A806" s="4"/>
+    </row>
+    <row r="807" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A807" s="4"/>
+    </row>
+    <row r="808" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A808" s="4"/>
+    </row>
+    <row r="809" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A809" s="4"/>
+    </row>
+    <row r="810" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A810" s="4"/>
+    </row>
+    <row r="811" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A811" s="4"/>
+    </row>
+    <row r="812" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A812" s="4"/>
+    </row>
+    <row r="813" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A813" s="4"/>
+    </row>
+    <row r="814" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A814" s="4"/>
+    </row>
+    <row r="815" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A815" s="4"/>
+    </row>
+    <row r="816" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A816" s="4"/>
+    </row>
+    <row r="817" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A817" s="4"/>
+    </row>
+    <row r="818" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A818" s="4"/>
+    </row>
+    <row r="819" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A819" s="4"/>
+    </row>
+    <row r="820" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A820" s="4"/>
+    </row>
+    <row r="821" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A821" s="4"/>
+    </row>
+    <row r="822" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A822" s="4"/>
+    </row>
+    <row r="823" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A823" s="4"/>
+    </row>
+    <row r="824" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A824" s="4"/>
+    </row>
+    <row r="825" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A825" s="4"/>
+    </row>
+    <row r="826" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A826" s="4"/>
+    </row>
+    <row r="827" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A827" s="4"/>
+    </row>
+    <row r="828" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A828" s="4"/>
+    </row>
+    <row r="829" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A829" s="4"/>
+    </row>
+    <row r="830" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A830" s="4"/>
+    </row>
+    <row r="831" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A831" s="4"/>
+    </row>
+    <row r="832" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A832" s="4"/>
+    </row>
+    <row r="833" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A833" s="4"/>
+    </row>
+    <row r="834" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A834" s="4"/>
+    </row>
+    <row r="835" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A835" s="4"/>
+    </row>
+    <row r="836" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A836" s="4"/>
+    </row>
+    <row r="837" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A837" s="4"/>
+    </row>
+    <row r="838" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A838" s="4"/>
+    </row>
+    <row r="839" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A839" s="4"/>
+    </row>
+    <row r="840" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A840" s="4"/>
+    </row>
+    <row r="841" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A841" s="4"/>
+    </row>
+    <row r="842" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A842" s="4"/>
+    </row>
+    <row r="843" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A843" s="4"/>
+    </row>
+    <row r="844" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A844" s="4"/>
+    </row>
+    <row r="845" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A845" s="4"/>
+    </row>
+    <row r="846" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A846" s="4"/>
+    </row>
+    <row r="847" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A847" s="4"/>
+    </row>
+    <row r="848" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A848" s="4"/>
+    </row>
+    <row r="849" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A849" s="4"/>
+    </row>
+    <row r="850" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A850" s="4"/>
+    </row>
+    <row r="851" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A851" s="4"/>
+    </row>
+    <row r="852" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A852" s="4"/>
+    </row>
+    <row r="853" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A853" s="4"/>
+    </row>
+    <row r="854" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A854" s="4"/>
+    </row>
+    <row r="855" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A855" s="4"/>
+    </row>
+    <row r="856" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A856" s="4"/>
+    </row>
+    <row r="857" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A857" s="4"/>
+    </row>
+    <row r="858" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A858" s="4"/>
+    </row>
+    <row r="859" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A859" s="4"/>
+    </row>
+    <row r="860" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A860" s="4"/>
+    </row>
+    <row r="861" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A861" s="4"/>
+    </row>
+    <row r="862" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A862" s="4"/>
+    </row>
+    <row r="863" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A863" s="4"/>
+    </row>
+    <row r="864" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A864" s="4"/>
+    </row>
+    <row r="865" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A865" s="4"/>
+    </row>
+    <row r="866" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A866" s="4"/>
+    </row>
+    <row r="867" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A867" s="4"/>
+    </row>
+    <row r="868" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A868" s="4"/>
+    </row>
+    <row r="869" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A869" s="4"/>
+    </row>
+    <row r="870" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A870" s="4"/>
+    </row>
+    <row r="871" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A871" s="4"/>
+    </row>
+    <row r="872" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A872" s="4"/>
+    </row>
+    <row r="873" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A873" s="4"/>
+    </row>
+    <row r="874" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A874" s="4"/>
+    </row>
+    <row r="875" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A875" s="4"/>
+    </row>
+    <row r="876" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A876" s="4"/>
+    </row>
+    <row r="877" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A877" s="4"/>
+    </row>
+    <row r="878" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A878" s="4"/>
+    </row>
+    <row r="879" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A879" s="4"/>
+    </row>
+    <row r="880" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A880" s="4"/>
+    </row>
+    <row r="881" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A881" s="4"/>
+    </row>
+    <row r="882" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A882" s="4"/>
+    </row>
+    <row r="883" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A883" s="4"/>
+    </row>
+    <row r="884" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A884" s="4"/>
+    </row>
+    <row r="885" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A885" s="4"/>
+    </row>
+    <row r="886" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A886" s="4"/>
+    </row>
+    <row r="887" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A887" s="4"/>
+    </row>
+    <row r="888" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A888" s="4"/>
+    </row>
+    <row r="889" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A889" s="4"/>
+    </row>
+    <row r="890" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A890" s="4"/>
+    </row>
+    <row r="891" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A891" s="4"/>
+    </row>
+    <row r="892" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A892" s="4"/>
+    </row>
+    <row r="893" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A893" s="4"/>
+    </row>
+    <row r="894" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A894" s="4"/>
+    </row>
+    <row r="895" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A895" s="4"/>
+    </row>
+    <row r="896" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A896" s="4"/>
+    </row>
+    <row r="897" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A897" s="4"/>
+    </row>
+    <row r="898" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A898" s="4"/>
+    </row>
+    <row r="899" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A899" s="4"/>
+    </row>
+    <row r="900" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A900" s="4"/>
+    </row>
+    <row r="901" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A901" s="4"/>
+    </row>
+    <row r="902" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A902" s="4"/>
+    </row>
+    <row r="903" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A903" s="4"/>
+    </row>
+    <row r="904" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A904" s="4"/>
+    </row>
+    <row r="905" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A905" s="4"/>
+    </row>
+    <row r="906" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A906" s="4"/>
+    </row>
+    <row r="907" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A907" s="4"/>
+    </row>
+    <row r="908" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A908" s="4"/>
+    </row>
+    <row r="909" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A909" s="4"/>
+    </row>
+    <row r="910" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A910" s="4"/>
+    </row>
+    <row r="911" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A911" s="4"/>
+    </row>
+    <row r="912" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A912" s="4"/>
+    </row>
+    <row r="913" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A913" s="4"/>
+    </row>
+    <row r="914" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A914" s="4"/>
+    </row>
+    <row r="915" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A915" s="4"/>
+    </row>
+    <row r="916" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A916" s="4"/>
+    </row>
+    <row r="917" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A917" s="4"/>
+    </row>
+    <row r="918" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A918" s="4"/>
+    </row>
+    <row r="919" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A919" s="4"/>
+    </row>
+    <row r="920" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A920" s="4"/>
+    </row>
+    <row r="921" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A921" s="4"/>
+    </row>
+    <row r="922" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A922" s="4"/>
+    </row>
+    <row r="923" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A923" s="4"/>
+    </row>
+    <row r="924" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A924" s="4"/>
+    </row>
+    <row r="925" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A925" s="4"/>
+    </row>
+    <row r="926" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A926" s="4"/>
+    </row>
+    <row r="927" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A927" s="4"/>
+    </row>
+    <row r="928" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A928" s="4"/>
+    </row>
+    <row r="929" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A929" s="4"/>
+    </row>
+    <row r="930" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A930" s="4"/>
+    </row>
+    <row r="931" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A931" s="4"/>
+    </row>
+    <row r="932" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A932" s="4"/>
+    </row>
+    <row r="933" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A933" s="4"/>
+    </row>
+    <row r="934" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A934" s="4"/>
+    </row>
+    <row r="935" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A935" s="4"/>
+    </row>
+    <row r="936" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A936" s="4"/>
+    </row>
+    <row r="937" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A937" s="4"/>
+    </row>
+    <row r="938" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A938" s="4"/>
+    </row>
+    <row r="939" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A939" s="4"/>
+    </row>
+    <row r="940" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A940" s="4"/>
+    </row>
+    <row r="941" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A941" s="4"/>
+    </row>
+    <row r="942" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A942" s="4"/>
+    </row>
+    <row r="943" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A943" s="4"/>
+    </row>
+    <row r="944" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A944" s="4"/>
+    </row>
+    <row r="945" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A945" s="4"/>
+    </row>
+    <row r="946" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A946" s="4"/>
+    </row>
+    <row r="947" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A947" s="4"/>
+    </row>
+    <row r="948" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A948" s="4"/>
+    </row>
+    <row r="949" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A949" s="4"/>
+    </row>
+    <row r="950" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A950" s="4"/>
+    </row>
+    <row r="951" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A951" s="4"/>
+    </row>
+    <row r="952" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A952" s="4"/>
+    </row>
+    <row r="953" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A953" s="4"/>
+    </row>
+    <row r="954" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A954" s="4"/>
+    </row>
+    <row r="955" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A955" s="4"/>
+    </row>
+    <row r="956" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A956" s="4"/>
+    </row>
+    <row r="957" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A957" s="4"/>
+    </row>
+    <row r="958" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A958" s="4"/>
+    </row>
+    <row r="959" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A959" s="4"/>
+    </row>
+    <row r="960" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A960" s="4"/>
+    </row>
+    <row r="961" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A961" s="4"/>
+    </row>
+    <row r="962" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A962" s="4"/>
+    </row>
+    <row r="963" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A963" s="4"/>
+    </row>
+    <row r="964" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A964" s="4"/>
+    </row>
+    <row r="965" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A965" s="4"/>
+    </row>
+    <row r="966" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A966" s="4"/>
+    </row>
+    <row r="967" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A967" s="4"/>
+    </row>
+    <row r="968" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A968" s="4"/>
+    </row>
+    <row r="969" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A969" s="4"/>
+    </row>
+    <row r="970" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A970" s="4"/>
+    </row>
+    <row r="971" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A971" s="4"/>
+    </row>
+    <row r="972" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A972" s="4"/>
+    </row>
+    <row r="973" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A973" s="4"/>
+    </row>
+    <row r="974" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A974" s="4"/>
+    </row>
+    <row r="975" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A975" s="4"/>
+    </row>
+    <row r="976" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A976" s="4"/>
+    </row>
+    <row r="977" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A977" s="4"/>
+    </row>
+    <row r="978" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A978" s="4"/>
+    </row>
+    <row r="979" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A979" s="4"/>
+    </row>
+    <row r="980" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A980" s="4"/>
+    </row>
+    <row r="981" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A981" s="4"/>
+    </row>
+    <row r="982" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A982" s="4"/>
+    </row>
+    <row r="983" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A983" s="4"/>
+    </row>
+    <row r="984" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A984" s="4"/>
+    </row>
+    <row r="985" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A985" s="4"/>
+    </row>
+    <row r="986" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A986" s="4"/>
+    </row>
+    <row r="987" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A987" s="4"/>
+    </row>
+    <row r="988" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A988" s="4"/>
+    </row>
+    <row r="989" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A989" s="4"/>
+    </row>
+    <row r="990" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A990" s="4"/>
+    </row>
+    <row r="991" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A991" s="4"/>
+    </row>
+    <row r="992" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A992" s="4"/>
+    </row>
+    <row r="993" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A993" s="4"/>
+    </row>
+    <row r="994" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A994" s="4"/>
+    </row>
+    <row r="995" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A995" s="4"/>
+    </row>
+    <row r="996" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A996" s="4"/>
+    </row>
+    <row r="997" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A997" s="4"/>
+    </row>
+    <row r="998" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A998" s="4"/>
+    </row>
+    <row r="999" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A999" s="4"/>
+    </row>
+    <row r="1000" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A1000" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{550D7409-88C4-468D-B7C2-154786EA112D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Put in Alt1 and Alt2
</commit_message>
<xml_diff>
--- a/CH-117 Add Index Column.xlsx
+++ b/CH-117 Add Index Column.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC7DD17-6EB3-42B9-B4BF-57CD0378D810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEC558A-8CD0-4402-AA1E-892687038954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt2" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -59,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="8">
   <si>
     <t>Question Table</t>
   </si>
@@ -92,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,10 +151,26 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +193,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEDF6D3"/>
         <bgColor rgb="FFEDF6D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -294,9 +326,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -328,21 +362,23 @@
     <xf numFmtId="3" fontId="7" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Intro_Hd" xfId="3" xr:uid="{966BB6FD-526C-4328-91B6-FA9886A197C8}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{F3743C4E-70CC-40A7-BA6D-2ED4C42B1503}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -702,6 +738,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="443" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{F25C954A-7ACA-45D4-8E0E-93874ED79422}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
@@ -722,19 +785,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="12"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="3"/>
@@ -4075,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37567A5-3451-4387-BA94-B2399B6069E6}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -4091,19 +4154,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="12"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="3"/>
@@ -4478,7 +4541,7 @@
     </row>
     <row r="18" spans="1:2" ht="14.4" customHeight="1">
       <c r="A18" s="4"/>
-      <c r="B18" s="15" cm="1">
+      <c r="B18" s="12" cm="1">
         <f t="array" ref="B18:B28">_xlfn.MAP(B3:B13,_xlfn.LAMBDA(_xlpm.x,COUNTIF(B3:_xlpm.x,_xlpm.x)))</f>
         <v>1</v>
       </c>
@@ -7471,4 +7534,3480 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E044E4CB-315B-4EB0-BC23-6433B041C3BC}">
+  <dimension ref="A1:Z1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" customWidth="1"/>
+    <col min="5" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="26" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="22.5" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9">
+        <v>100</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10">
+        <v>100</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10">
+        <v>45</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10">
+        <v>88</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9">
+        <v>49</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="10">
+        <v>49</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" ht="14.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="10">
+        <v>43</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10">
+        <v>76</v>
+      </c>
+      <c r="G8" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9">
+        <v>84</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="10">
+        <v>84</v>
+      </c>
+      <c r="G9" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="10">
+        <v>40</v>
+      </c>
+      <c r="G10" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10">
+        <v>69</v>
+      </c>
+      <c r="G11" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="10">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="10">
+        <v>22</v>
+      </c>
+      <c r="G13" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.4">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.4">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.4" customHeight="1">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.4">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A18" s="4"/>
+      <c r="B18" s="12" t="str" cm="1">
+        <f t="array" ref="B18:D28">_xlfn.HSTACK(
+    B3:C13,
+    _xlfn.MAP(
+        B3:B13,
+        _xlfn.LAMBDA(_xlpm.b,
+            SUM(N(+B3:_xlpm.b = _xlpm.b))
+        )
+    )
+)</f>
+        <v>A</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A19" s="4"/>
+      <c r="B19" t="str">
+        <v>A</v>
+      </c>
+      <c r="C19">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" t="str">
+        <v>A</v>
+      </c>
+      <c r="C20">
+        <v>88</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" t="str">
+        <v>B</v>
+      </c>
+      <c r="C21">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A22" s="4"/>
+      <c r="B22" t="str">
+        <v>B</v>
+      </c>
+      <c r="C22">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23" t="str">
+        <v>A</v>
+      </c>
+      <c r="C23">
+        <v>76</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24" t="str">
+        <v>B</v>
+      </c>
+      <c r="C24">
+        <v>84</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="B25" t="str">
+        <v>A</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A26" s="4"/>
+      <c r="B26" t="str">
+        <v>A</v>
+      </c>
+      <c r="C26">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A27" s="4"/>
+      <c r="B27" t="str">
+        <v>B</v>
+      </c>
+      <c r="C27">
+        <v>14</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.4" customHeight="1">
+      <c r="A28" s="4"/>
+      <c r="B28" t="str">
+        <v>B</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A36" s="4"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A91" s="4"/>
+    </row>
+    <row r="92" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A92" s="4"/>
+    </row>
+    <row r="93" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A94" s="4"/>
+    </row>
+    <row r="95" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A96" s="4"/>
+    </row>
+    <row r="97" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A99" s="4"/>
+    </row>
+    <row r="100" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A101" s="4"/>
+    </row>
+    <row r="102" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A102" s="4"/>
+    </row>
+    <row r="103" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A103" s="4"/>
+    </row>
+    <row r="104" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A104" s="4"/>
+    </row>
+    <row r="105" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A105" s="4"/>
+    </row>
+    <row r="106" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A106" s="4"/>
+    </row>
+    <row r="107" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A107" s="4"/>
+    </row>
+    <row r="108" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A108" s="4"/>
+    </row>
+    <row r="109" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A109" s="4"/>
+    </row>
+    <row r="110" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A110" s="4"/>
+    </row>
+    <row r="111" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A111" s="4"/>
+    </row>
+    <row r="112" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A112" s="4"/>
+    </row>
+    <row r="113" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A114" s="4"/>
+    </row>
+    <row r="115" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A116" s="4"/>
+    </row>
+    <row r="117" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A118" s="4"/>
+    </row>
+    <row r="119" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A120" s="4"/>
+    </row>
+    <row r="121" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A121" s="4"/>
+    </row>
+    <row r="122" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A122" s="4"/>
+    </row>
+    <row r="123" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A123" s="4"/>
+    </row>
+    <row r="124" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A124" s="4"/>
+    </row>
+    <row r="125" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A125" s="4"/>
+    </row>
+    <row r="126" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A126" s="4"/>
+    </row>
+    <row r="127" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A127" s="4"/>
+    </row>
+    <row r="128" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A128" s="4"/>
+    </row>
+    <row r="129" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A129" s="4"/>
+    </row>
+    <row r="130" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A130" s="4"/>
+    </row>
+    <row r="131" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A132" s="4"/>
+    </row>
+    <row r="133" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A133" s="4"/>
+    </row>
+    <row r="134" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A134" s="4"/>
+    </row>
+    <row r="135" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A135" s="4"/>
+    </row>
+    <row r="136" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A136" s="4"/>
+    </row>
+    <row r="137" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A137" s="4"/>
+    </row>
+    <row r="138" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A138" s="4"/>
+    </row>
+    <row r="139" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A139" s="4"/>
+    </row>
+    <row r="140" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A140" s="4"/>
+    </row>
+    <row r="141" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A141" s="4"/>
+    </row>
+    <row r="142" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A142" s="4"/>
+    </row>
+    <row r="143" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A143" s="4"/>
+    </row>
+    <row r="144" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A144" s="4"/>
+    </row>
+    <row r="145" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A145" s="4"/>
+    </row>
+    <row r="146" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A146" s="4"/>
+    </row>
+    <row r="147" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A147" s="4"/>
+    </row>
+    <row r="148" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A148" s="4"/>
+    </row>
+    <row r="149" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A149" s="4"/>
+    </row>
+    <row r="150" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A150" s="4"/>
+    </row>
+    <row r="151" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A151" s="4"/>
+    </row>
+    <row r="152" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A152" s="4"/>
+    </row>
+    <row r="153" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A153" s="4"/>
+    </row>
+    <row r="154" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A154" s="4"/>
+    </row>
+    <row r="155" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A155" s="4"/>
+    </row>
+    <row r="156" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A156" s="4"/>
+    </row>
+    <row r="157" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A157" s="4"/>
+    </row>
+    <row r="158" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A158" s="4"/>
+    </row>
+    <row r="159" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A159" s="4"/>
+    </row>
+    <row r="160" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A160" s="4"/>
+    </row>
+    <row r="161" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A161" s="4"/>
+    </row>
+    <row r="162" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A162" s="4"/>
+    </row>
+    <row r="163" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A163" s="4"/>
+    </row>
+    <row r="164" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A164" s="4"/>
+    </row>
+    <row r="165" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A165" s="4"/>
+    </row>
+    <row r="166" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A166" s="4"/>
+    </row>
+    <row r="167" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A167" s="4"/>
+    </row>
+    <row r="168" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A168" s="4"/>
+    </row>
+    <row r="169" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A169" s="4"/>
+    </row>
+    <row r="170" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A170" s="4"/>
+    </row>
+    <row r="171" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A171" s="4"/>
+    </row>
+    <row r="172" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A172" s="4"/>
+    </row>
+    <row r="173" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A173" s="4"/>
+    </row>
+    <row r="174" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A174" s="4"/>
+    </row>
+    <row r="175" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A175" s="4"/>
+    </row>
+    <row r="176" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A176" s="4"/>
+    </row>
+    <row r="177" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A177" s="4"/>
+    </row>
+    <row r="178" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A178" s="4"/>
+    </row>
+    <row r="179" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A179" s="4"/>
+    </row>
+    <row r="180" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A180" s="4"/>
+    </row>
+    <row r="181" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A181" s="4"/>
+    </row>
+    <row r="182" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A182" s="4"/>
+    </row>
+    <row r="183" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A183" s="4"/>
+    </row>
+    <row r="184" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A184" s="4"/>
+    </row>
+    <row r="185" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A185" s="4"/>
+    </row>
+    <row r="186" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A186" s="4"/>
+    </row>
+    <row r="187" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A187" s="4"/>
+    </row>
+    <row r="188" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A188" s="4"/>
+    </row>
+    <row r="189" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A189" s="4"/>
+    </row>
+    <row r="190" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A190" s="4"/>
+    </row>
+    <row r="191" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A191" s="4"/>
+    </row>
+    <row r="192" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A192" s="4"/>
+    </row>
+    <row r="193" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A193" s="4"/>
+    </row>
+    <row r="194" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A194" s="4"/>
+    </row>
+    <row r="195" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A195" s="4"/>
+    </row>
+    <row r="196" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A196" s="4"/>
+    </row>
+    <row r="197" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A197" s="4"/>
+    </row>
+    <row r="198" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A198" s="4"/>
+    </row>
+    <row r="199" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A199" s="4"/>
+    </row>
+    <row r="200" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A200" s="4"/>
+    </row>
+    <row r="201" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A201" s="4"/>
+    </row>
+    <row r="202" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A202" s="4"/>
+    </row>
+    <row r="203" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A203" s="4"/>
+    </row>
+    <row r="204" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A204" s="4"/>
+    </row>
+    <row r="205" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A205" s="4"/>
+    </row>
+    <row r="206" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A206" s="4"/>
+    </row>
+    <row r="207" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A207" s="4"/>
+    </row>
+    <row r="208" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A208" s="4"/>
+    </row>
+    <row r="209" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A209" s="4"/>
+    </row>
+    <row r="210" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A210" s="4"/>
+    </row>
+    <row r="211" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A211" s="4"/>
+    </row>
+    <row r="212" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A212" s="4"/>
+    </row>
+    <row r="213" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A213" s="4"/>
+    </row>
+    <row r="214" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A214" s="4"/>
+    </row>
+    <row r="215" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A215" s="4"/>
+    </row>
+    <row r="216" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A216" s="4"/>
+    </row>
+    <row r="217" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A217" s="4"/>
+    </row>
+    <row r="218" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A218" s="4"/>
+    </row>
+    <row r="219" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A219" s="4"/>
+    </row>
+    <row r="220" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A220" s="4"/>
+    </row>
+    <row r="221" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A221" s="4"/>
+    </row>
+    <row r="222" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A222" s="4"/>
+    </row>
+    <row r="223" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A223" s="4"/>
+    </row>
+    <row r="224" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A224" s="4"/>
+    </row>
+    <row r="225" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A225" s="4"/>
+    </row>
+    <row r="226" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A226" s="4"/>
+    </row>
+    <row r="227" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A227" s="4"/>
+    </row>
+    <row r="228" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A228" s="4"/>
+    </row>
+    <row r="229" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A229" s="4"/>
+    </row>
+    <row r="230" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A230" s="4"/>
+    </row>
+    <row r="231" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A231" s="4"/>
+    </row>
+    <row r="232" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A232" s="4"/>
+    </row>
+    <row r="233" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A233" s="4"/>
+    </row>
+    <row r="234" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A234" s="4"/>
+    </row>
+    <row r="235" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A235" s="4"/>
+    </row>
+    <row r="236" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A236" s="4"/>
+    </row>
+    <row r="237" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A237" s="4"/>
+    </row>
+    <row r="238" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A238" s="4"/>
+    </row>
+    <row r="239" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A239" s="4"/>
+    </row>
+    <row r="240" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A240" s="4"/>
+    </row>
+    <row r="241" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A241" s="4"/>
+    </row>
+    <row r="242" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A242" s="4"/>
+    </row>
+    <row r="243" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A243" s="4"/>
+    </row>
+    <row r="244" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A244" s="4"/>
+    </row>
+    <row r="245" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A245" s="4"/>
+    </row>
+    <row r="246" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A246" s="4"/>
+    </row>
+    <row r="247" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A247" s="4"/>
+    </row>
+    <row r="248" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A248" s="4"/>
+    </row>
+    <row r="249" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A249" s="4"/>
+    </row>
+    <row r="250" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A250" s="4"/>
+    </row>
+    <row r="251" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A251" s="4"/>
+    </row>
+    <row r="252" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A252" s="4"/>
+    </row>
+    <row r="253" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A253" s="4"/>
+    </row>
+    <row r="254" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A254" s="4"/>
+    </row>
+    <row r="255" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A255" s="4"/>
+    </row>
+    <row r="256" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A256" s="4"/>
+    </row>
+    <row r="257" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A257" s="4"/>
+    </row>
+    <row r="258" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A258" s="4"/>
+    </row>
+    <row r="259" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A259" s="4"/>
+    </row>
+    <row r="260" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A260" s="4"/>
+    </row>
+    <row r="261" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A261" s="4"/>
+    </row>
+    <row r="262" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A262" s="4"/>
+    </row>
+    <row r="263" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A263" s="4"/>
+    </row>
+    <row r="264" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A264" s="4"/>
+    </row>
+    <row r="265" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A265" s="4"/>
+    </row>
+    <row r="266" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A266" s="4"/>
+    </row>
+    <row r="267" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A267" s="4"/>
+    </row>
+    <row r="268" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A268" s="4"/>
+    </row>
+    <row r="269" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A269" s="4"/>
+    </row>
+    <row r="270" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A270" s="4"/>
+    </row>
+    <row r="271" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A271" s="4"/>
+    </row>
+    <row r="272" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A272" s="4"/>
+    </row>
+    <row r="273" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A273" s="4"/>
+    </row>
+    <row r="274" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A274" s="4"/>
+    </row>
+    <row r="275" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A275" s="4"/>
+    </row>
+    <row r="276" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A276" s="4"/>
+    </row>
+    <row r="277" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A277" s="4"/>
+    </row>
+    <row r="278" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A278" s="4"/>
+    </row>
+    <row r="279" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A279" s="4"/>
+    </row>
+    <row r="280" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A280" s="4"/>
+    </row>
+    <row r="281" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A281" s="4"/>
+    </row>
+    <row r="282" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A282" s="4"/>
+    </row>
+    <row r="283" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A283" s="4"/>
+    </row>
+    <row r="284" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A284" s="4"/>
+    </row>
+    <row r="285" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A285" s="4"/>
+    </row>
+    <row r="286" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A286" s="4"/>
+    </row>
+    <row r="287" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A287" s="4"/>
+    </row>
+    <row r="288" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A288" s="4"/>
+    </row>
+    <row r="289" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A289" s="4"/>
+    </row>
+    <row r="290" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A290" s="4"/>
+    </row>
+    <row r="291" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A291" s="4"/>
+    </row>
+    <row r="292" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A292" s="4"/>
+    </row>
+    <row r="293" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A293" s="4"/>
+    </row>
+    <row r="294" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A294" s="4"/>
+    </row>
+    <row r="295" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A295" s="4"/>
+    </row>
+    <row r="296" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A296" s="4"/>
+    </row>
+    <row r="297" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A297" s="4"/>
+    </row>
+    <row r="298" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A298" s="4"/>
+    </row>
+    <row r="299" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A299" s="4"/>
+    </row>
+    <row r="300" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A300" s="4"/>
+    </row>
+    <row r="301" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A301" s="4"/>
+    </row>
+    <row r="302" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A302" s="4"/>
+    </row>
+    <row r="303" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A303" s="4"/>
+    </row>
+    <row r="304" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A304" s="4"/>
+    </row>
+    <row r="305" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A305" s="4"/>
+    </row>
+    <row r="306" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A306" s="4"/>
+    </row>
+    <row r="307" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A307" s="4"/>
+    </row>
+    <row r="308" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A308" s="4"/>
+    </row>
+    <row r="309" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A309" s="4"/>
+    </row>
+    <row r="310" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A310" s="4"/>
+    </row>
+    <row r="311" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A311" s="4"/>
+    </row>
+    <row r="312" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A312" s="4"/>
+    </row>
+    <row r="313" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A313" s="4"/>
+    </row>
+    <row r="314" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A314" s="4"/>
+    </row>
+    <row r="315" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A315" s="4"/>
+    </row>
+    <row r="316" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A316" s="4"/>
+    </row>
+    <row r="317" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A317" s="4"/>
+    </row>
+    <row r="318" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A318" s="4"/>
+    </row>
+    <row r="319" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A319" s="4"/>
+    </row>
+    <row r="320" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A320" s="4"/>
+    </row>
+    <row r="321" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A321" s="4"/>
+    </row>
+    <row r="322" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A322" s="4"/>
+    </row>
+    <row r="323" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A323" s="4"/>
+    </row>
+    <row r="324" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A324" s="4"/>
+    </row>
+    <row r="325" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A325" s="4"/>
+    </row>
+    <row r="326" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A326" s="4"/>
+    </row>
+    <row r="327" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A327" s="4"/>
+    </row>
+    <row r="328" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A328" s="4"/>
+    </row>
+    <row r="329" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A329" s="4"/>
+    </row>
+    <row r="330" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A330" s="4"/>
+    </row>
+    <row r="331" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A331" s="4"/>
+    </row>
+    <row r="332" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A332" s="4"/>
+    </row>
+    <row r="333" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A333" s="4"/>
+    </row>
+    <row r="334" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A334" s="4"/>
+    </row>
+    <row r="335" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A335" s="4"/>
+    </row>
+    <row r="336" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A336" s="4"/>
+    </row>
+    <row r="337" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A337" s="4"/>
+    </row>
+    <row r="338" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A338" s="4"/>
+    </row>
+    <row r="339" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A339" s="4"/>
+    </row>
+    <row r="340" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A340" s="4"/>
+    </row>
+    <row r="341" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A341" s="4"/>
+    </row>
+    <row r="342" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A342" s="4"/>
+    </row>
+    <row r="343" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A343" s="4"/>
+    </row>
+    <row r="344" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A344" s="4"/>
+    </row>
+    <row r="345" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A345" s="4"/>
+    </row>
+    <row r="346" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A346" s="4"/>
+    </row>
+    <row r="347" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A347" s="4"/>
+    </row>
+    <row r="348" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A348" s="4"/>
+    </row>
+    <row r="349" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A349" s="4"/>
+    </row>
+    <row r="350" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A350" s="4"/>
+    </row>
+    <row r="351" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A351" s="4"/>
+    </row>
+    <row r="352" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A352" s="4"/>
+    </row>
+    <row r="353" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A353" s="4"/>
+    </row>
+    <row r="354" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A354" s="4"/>
+    </row>
+    <row r="355" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A355" s="4"/>
+    </row>
+    <row r="356" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A356" s="4"/>
+    </row>
+    <row r="357" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A357" s="4"/>
+    </row>
+    <row r="358" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A358" s="4"/>
+    </row>
+    <row r="359" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A359" s="4"/>
+    </row>
+    <row r="360" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A360" s="4"/>
+    </row>
+    <row r="361" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A361" s="4"/>
+    </row>
+    <row r="362" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A362" s="4"/>
+    </row>
+    <row r="363" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A363" s="4"/>
+    </row>
+    <row r="364" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A364" s="4"/>
+    </row>
+    <row r="365" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A365" s="4"/>
+    </row>
+    <row r="366" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A366" s="4"/>
+    </row>
+    <row r="367" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A367" s="4"/>
+    </row>
+    <row r="368" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A368" s="4"/>
+    </row>
+    <row r="369" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A369" s="4"/>
+    </row>
+    <row r="370" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A370" s="4"/>
+    </row>
+    <row r="371" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A371" s="4"/>
+    </row>
+    <row r="372" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A372" s="4"/>
+    </row>
+    <row r="373" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A373" s="4"/>
+    </row>
+    <row r="374" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A374" s="4"/>
+    </row>
+    <row r="375" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A375" s="4"/>
+    </row>
+    <row r="376" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A376" s="4"/>
+    </row>
+    <row r="377" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A377" s="4"/>
+    </row>
+    <row r="378" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A378" s="4"/>
+    </row>
+    <row r="379" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A379" s="4"/>
+    </row>
+    <row r="380" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A380" s="4"/>
+    </row>
+    <row r="381" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A381" s="4"/>
+    </row>
+    <row r="382" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A382" s="4"/>
+    </row>
+    <row r="383" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A383" s="4"/>
+    </row>
+    <row r="384" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A384" s="4"/>
+    </row>
+    <row r="385" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A385" s="4"/>
+    </row>
+    <row r="386" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A386" s="4"/>
+    </row>
+    <row r="387" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A387" s="4"/>
+    </row>
+    <row r="388" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A388" s="4"/>
+    </row>
+    <row r="389" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A389" s="4"/>
+    </row>
+    <row r="390" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A390" s="4"/>
+    </row>
+    <row r="391" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A391" s="4"/>
+    </row>
+    <row r="392" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A392" s="4"/>
+    </row>
+    <row r="393" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A393" s="4"/>
+    </row>
+    <row r="394" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A394" s="4"/>
+    </row>
+    <row r="395" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A395" s="4"/>
+    </row>
+    <row r="396" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A396" s="4"/>
+    </row>
+    <row r="397" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A397" s="4"/>
+    </row>
+    <row r="398" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A398" s="4"/>
+    </row>
+    <row r="399" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A399" s="4"/>
+    </row>
+    <row r="400" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A400" s="4"/>
+    </row>
+    <row r="401" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A401" s="4"/>
+    </row>
+    <row r="402" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A402" s="4"/>
+    </row>
+    <row r="403" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A403" s="4"/>
+    </row>
+    <row r="404" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A404" s="4"/>
+    </row>
+    <row r="405" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A405" s="4"/>
+    </row>
+    <row r="406" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A406" s="4"/>
+    </row>
+    <row r="407" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A407" s="4"/>
+    </row>
+    <row r="408" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A408" s="4"/>
+    </row>
+    <row r="409" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A409" s="4"/>
+    </row>
+    <row r="410" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A410" s="4"/>
+    </row>
+    <row r="411" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A411" s="4"/>
+    </row>
+    <row r="412" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A412" s="4"/>
+    </row>
+    <row r="413" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A413" s="4"/>
+    </row>
+    <row r="414" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A414" s="4"/>
+    </row>
+    <row r="415" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A415" s="4"/>
+    </row>
+    <row r="416" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A416" s="4"/>
+    </row>
+    <row r="417" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A417" s="4"/>
+    </row>
+    <row r="418" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A418" s="4"/>
+    </row>
+    <row r="419" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A419" s="4"/>
+    </row>
+    <row r="420" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A420" s="4"/>
+    </row>
+    <row r="421" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A421" s="4"/>
+    </row>
+    <row r="422" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A422" s="4"/>
+    </row>
+    <row r="423" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A423" s="4"/>
+    </row>
+    <row r="424" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A424" s="4"/>
+    </row>
+    <row r="425" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A425" s="4"/>
+    </row>
+    <row r="426" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A426" s="4"/>
+    </row>
+    <row r="427" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A427" s="4"/>
+    </row>
+    <row r="428" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A428" s="4"/>
+    </row>
+    <row r="429" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A429" s="4"/>
+    </row>
+    <row r="430" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A430" s="4"/>
+    </row>
+    <row r="431" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A431" s="4"/>
+    </row>
+    <row r="432" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A432" s="4"/>
+    </row>
+    <row r="433" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A433" s="4"/>
+    </row>
+    <row r="434" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A434" s="4"/>
+    </row>
+    <row r="435" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A435" s="4"/>
+    </row>
+    <row r="436" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A436" s="4"/>
+    </row>
+    <row r="437" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A437" s="4"/>
+    </row>
+    <row r="438" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A438" s="4"/>
+    </row>
+    <row r="439" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A439" s="4"/>
+    </row>
+    <row r="440" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A440" s="4"/>
+    </row>
+    <row r="441" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A441" s="4"/>
+    </row>
+    <row r="442" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A442" s="4"/>
+    </row>
+    <row r="443" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A443" s="4"/>
+    </row>
+    <row r="444" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A444" s="4"/>
+    </row>
+    <row r="445" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A445" s="4"/>
+    </row>
+    <row r="446" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A446" s="4"/>
+    </row>
+    <row r="447" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A447" s="4"/>
+    </row>
+    <row r="448" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A448" s="4"/>
+    </row>
+    <row r="449" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A449" s="4"/>
+    </row>
+    <row r="450" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A450" s="4"/>
+    </row>
+    <row r="451" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A451" s="4"/>
+    </row>
+    <row r="452" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A452" s="4"/>
+    </row>
+    <row r="453" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A453" s="4"/>
+    </row>
+    <row r="454" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A454" s="4"/>
+    </row>
+    <row r="455" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A455" s="4"/>
+    </row>
+    <row r="456" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A456" s="4"/>
+    </row>
+    <row r="457" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A457" s="4"/>
+    </row>
+    <row r="458" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A458" s="4"/>
+    </row>
+    <row r="459" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A459" s="4"/>
+    </row>
+    <row r="460" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A460" s="4"/>
+    </row>
+    <row r="461" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A461" s="4"/>
+    </row>
+    <row r="462" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A462" s="4"/>
+    </row>
+    <row r="463" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A463" s="4"/>
+    </row>
+    <row r="464" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A464" s="4"/>
+    </row>
+    <row r="465" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A465" s="4"/>
+    </row>
+    <row r="466" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A466" s="4"/>
+    </row>
+    <row r="467" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A467" s="4"/>
+    </row>
+    <row r="468" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A468" s="4"/>
+    </row>
+    <row r="469" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A469" s="4"/>
+    </row>
+    <row r="470" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A470" s="4"/>
+    </row>
+    <row r="471" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A471" s="4"/>
+    </row>
+    <row r="472" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A472" s="4"/>
+    </row>
+    <row r="473" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A473" s="4"/>
+    </row>
+    <row r="474" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A474" s="4"/>
+    </row>
+    <row r="475" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A475" s="4"/>
+    </row>
+    <row r="476" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A476" s="4"/>
+    </row>
+    <row r="477" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A477" s="4"/>
+    </row>
+    <row r="478" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A478" s="4"/>
+    </row>
+    <row r="479" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A479" s="4"/>
+    </row>
+    <row r="480" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A480" s="4"/>
+    </row>
+    <row r="481" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A481" s="4"/>
+    </row>
+    <row r="482" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A482" s="4"/>
+    </row>
+    <row r="483" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A483" s="4"/>
+    </row>
+    <row r="484" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A484" s="4"/>
+    </row>
+    <row r="485" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A485" s="4"/>
+    </row>
+    <row r="486" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A486" s="4"/>
+    </row>
+    <row r="487" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A487" s="4"/>
+    </row>
+    <row r="488" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A488" s="4"/>
+    </row>
+    <row r="489" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A489" s="4"/>
+    </row>
+    <row r="490" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A490" s="4"/>
+    </row>
+    <row r="491" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A491" s="4"/>
+    </row>
+    <row r="492" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A492" s="4"/>
+    </row>
+    <row r="493" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A493" s="4"/>
+    </row>
+    <row r="494" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A494" s="4"/>
+    </row>
+    <row r="495" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A495" s="4"/>
+    </row>
+    <row r="496" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A496" s="4"/>
+    </row>
+    <row r="497" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A497" s="4"/>
+    </row>
+    <row r="498" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A498" s="4"/>
+    </row>
+    <row r="499" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A499" s="4"/>
+    </row>
+    <row r="500" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A500" s="4"/>
+    </row>
+    <row r="501" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A501" s="4"/>
+    </row>
+    <row r="502" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A502" s="4"/>
+    </row>
+    <row r="503" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A503" s="4"/>
+    </row>
+    <row r="504" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A504" s="4"/>
+    </row>
+    <row r="505" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A505" s="4"/>
+    </row>
+    <row r="506" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A506" s="4"/>
+    </row>
+    <row r="507" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A507" s="4"/>
+    </row>
+    <row r="508" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A508" s="4"/>
+    </row>
+    <row r="509" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A509" s="4"/>
+    </row>
+    <row r="510" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A510" s="4"/>
+    </row>
+    <row r="511" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A511" s="4"/>
+    </row>
+    <row r="512" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A512" s="4"/>
+    </row>
+    <row r="513" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A513" s="4"/>
+    </row>
+    <row r="514" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A514" s="4"/>
+    </row>
+    <row r="515" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A515" s="4"/>
+    </row>
+    <row r="516" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A516" s="4"/>
+    </row>
+    <row r="517" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A517" s="4"/>
+    </row>
+    <row r="518" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A518" s="4"/>
+    </row>
+    <row r="519" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A519" s="4"/>
+    </row>
+    <row r="520" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A520" s="4"/>
+    </row>
+    <row r="521" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A521" s="4"/>
+    </row>
+    <row r="522" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A522" s="4"/>
+    </row>
+    <row r="523" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A523" s="4"/>
+    </row>
+    <row r="524" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A524" s="4"/>
+    </row>
+    <row r="525" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A525" s="4"/>
+    </row>
+    <row r="526" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A526" s="4"/>
+    </row>
+    <row r="527" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A527" s="4"/>
+    </row>
+    <row r="528" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A528" s="4"/>
+    </row>
+    <row r="529" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A529" s="4"/>
+    </row>
+    <row r="530" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A530" s="4"/>
+    </row>
+    <row r="531" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A531" s="4"/>
+    </row>
+    <row r="532" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A532" s="4"/>
+    </row>
+    <row r="533" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A533" s="4"/>
+    </row>
+    <row r="534" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A534" s="4"/>
+    </row>
+    <row r="535" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A535" s="4"/>
+    </row>
+    <row r="536" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A536" s="4"/>
+    </row>
+    <row r="537" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A537" s="4"/>
+    </row>
+    <row r="538" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A538" s="4"/>
+    </row>
+    <row r="539" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A539" s="4"/>
+    </row>
+    <row r="540" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A540" s="4"/>
+    </row>
+    <row r="541" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A541" s="4"/>
+    </row>
+    <row r="542" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A542" s="4"/>
+    </row>
+    <row r="543" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A543" s="4"/>
+    </row>
+    <row r="544" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A544" s="4"/>
+    </row>
+    <row r="545" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A545" s="4"/>
+    </row>
+    <row r="546" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A546" s="4"/>
+    </row>
+    <row r="547" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A547" s="4"/>
+    </row>
+    <row r="548" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A548" s="4"/>
+    </row>
+    <row r="549" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A549" s="4"/>
+    </row>
+    <row r="550" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A550" s="4"/>
+    </row>
+    <row r="551" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A551" s="4"/>
+    </row>
+    <row r="552" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A552" s="4"/>
+    </row>
+    <row r="553" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A553" s="4"/>
+    </row>
+    <row r="554" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A554" s="4"/>
+    </row>
+    <row r="555" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A555" s="4"/>
+    </row>
+    <row r="556" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A556" s="4"/>
+    </row>
+    <row r="557" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A557" s="4"/>
+    </row>
+    <row r="558" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A558" s="4"/>
+    </row>
+    <row r="559" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A559" s="4"/>
+    </row>
+    <row r="560" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A560" s="4"/>
+    </row>
+    <row r="561" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A561" s="4"/>
+    </row>
+    <row r="562" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A562" s="4"/>
+    </row>
+    <row r="563" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A563" s="4"/>
+    </row>
+    <row r="564" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A564" s="4"/>
+    </row>
+    <row r="565" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A565" s="4"/>
+    </row>
+    <row r="566" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A566" s="4"/>
+    </row>
+    <row r="567" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A567" s="4"/>
+    </row>
+    <row r="568" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A568" s="4"/>
+    </row>
+    <row r="569" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A569" s="4"/>
+    </row>
+    <row r="570" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A570" s="4"/>
+    </row>
+    <row r="571" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A571" s="4"/>
+    </row>
+    <row r="572" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A572" s="4"/>
+    </row>
+    <row r="573" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A573" s="4"/>
+    </row>
+    <row r="574" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A574" s="4"/>
+    </row>
+    <row r="575" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A575" s="4"/>
+    </row>
+    <row r="576" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A576" s="4"/>
+    </row>
+    <row r="577" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A577" s="4"/>
+    </row>
+    <row r="578" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A578" s="4"/>
+    </row>
+    <row r="579" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A579" s="4"/>
+    </row>
+    <row r="580" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A580" s="4"/>
+    </row>
+    <row r="581" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A581" s="4"/>
+    </row>
+    <row r="582" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A582" s="4"/>
+    </row>
+    <row r="583" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A583" s="4"/>
+    </row>
+    <row r="584" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A584" s="4"/>
+    </row>
+    <row r="585" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A585" s="4"/>
+    </row>
+    <row r="586" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A586" s="4"/>
+    </row>
+    <row r="587" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A587" s="4"/>
+    </row>
+    <row r="588" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A588" s="4"/>
+    </row>
+    <row r="589" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A589" s="4"/>
+    </row>
+    <row r="590" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A590" s="4"/>
+    </row>
+    <row r="591" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A591" s="4"/>
+    </row>
+    <row r="592" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A592" s="4"/>
+    </row>
+    <row r="593" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A593" s="4"/>
+    </row>
+    <row r="594" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A594" s="4"/>
+    </row>
+    <row r="595" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A595" s="4"/>
+    </row>
+    <row r="596" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A596" s="4"/>
+    </row>
+    <row r="597" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A597" s="4"/>
+    </row>
+    <row r="598" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A598" s="4"/>
+    </row>
+    <row r="599" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A599" s="4"/>
+    </row>
+    <row r="600" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A600" s="4"/>
+    </row>
+    <row r="601" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A601" s="4"/>
+    </row>
+    <row r="602" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A602" s="4"/>
+    </row>
+    <row r="603" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A603" s="4"/>
+    </row>
+    <row r="604" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A604" s="4"/>
+    </row>
+    <row r="605" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A605" s="4"/>
+    </row>
+    <row r="606" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A606" s="4"/>
+    </row>
+    <row r="607" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A607" s="4"/>
+    </row>
+    <row r="608" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A608" s="4"/>
+    </row>
+    <row r="609" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A609" s="4"/>
+    </row>
+    <row r="610" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A610" s="4"/>
+    </row>
+    <row r="611" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A611" s="4"/>
+    </row>
+    <row r="612" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A612" s="4"/>
+    </row>
+    <row r="613" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A613" s="4"/>
+    </row>
+    <row r="614" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A614" s="4"/>
+    </row>
+    <row r="615" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A615" s="4"/>
+    </row>
+    <row r="616" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A616" s="4"/>
+    </row>
+    <row r="617" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A617" s="4"/>
+    </row>
+    <row r="618" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A618" s="4"/>
+    </row>
+    <row r="619" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A619" s="4"/>
+    </row>
+    <row r="620" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A620" s="4"/>
+    </row>
+    <row r="621" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A621" s="4"/>
+    </row>
+    <row r="622" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A622" s="4"/>
+    </row>
+    <row r="623" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A623" s="4"/>
+    </row>
+    <row r="624" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A624" s="4"/>
+    </row>
+    <row r="625" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A625" s="4"/>
+    </row>
+    <row r="626" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A626" s="4"/>
+    </row>
+    <row r="627" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A627" s="4"/>
+    </row>
+    <row r="628" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A628" s="4"/>
+    </row>
+    <row r="629" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A629" s="4"/>
+    </row>
+    <row r="630" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A630" s="4"/>
+    </row>
+    <row r="631" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A631" s="4"/>
+    </row>
+    <row r="632" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A632" s="4"/>
+    </row>
+    <row r="633" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A633" s="4"/>
+    </row>
+    <row r="634" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A634" s="4"/>
+    </row>
+    <row r="635" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A635" s="4"/>
+    </row>
+    <row r="636" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A636" s="4"/>
+    </row>
+    <row r="637" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A637" s="4"/>
+    </row>
+    <row r="638" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A638" s="4"/>
+    </row>
+    <row r="639" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A639" s="4"/>
+    </row>
+    <row r="640" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A640" s="4"/>
+    </row>
+    <row r="641" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A641" s="4"/>
+    </row>
+    <row r="642" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A642" s="4"/>
+    </row>
+    <row r="643" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A643" s="4"/>
+    </row>
+    <row r="644" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A644" s="4"/>
+    </row>
+    <row r="645" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A645" s="4"/>
+    </row>
+    <row r="646" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A646" s="4"/>
+    </row>
+    <row r="647" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A647" s="4"/>
+    </row>
+    <row r="648" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A648" s="4"/>
+    </row>
+    <row r="649" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A649" s="4"/>
+    </row>
+    <row r="650" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A650" s="4"/>
+    </row>
+    <row r="651" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A651" s="4"/>
+    </row>
+    <row r="652" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A652" s="4"/>
+    </row>
+    <row r="653" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A653" s="4"/>
+    </row>
+    <row r="654" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A654" s="4"/>
+    </row>
+    <row r="655" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A655" s="4"/>
+    </row>
+    <row r="656" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A656" s="4"/>
+    </row>
+    <row r="657" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A657" s="4"/>
+    </row>
+    <row r="658" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A658" s="4"/>
+    </row>
+    <row r="659" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A659" s="4"/>
+    </row>
+    <row r="660" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A660" s="4"/>
+    </row>
+    <row r="661" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A661" s="4"/>
+    </row>
+    <row r="662" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A662" s="4"/>
+    </row>
+    <row r="663" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A663" s="4"/>
+    </row>
+    <row r="664" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A664" s="4"/>
+    </row>
+    <row r="665" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A665" s="4"/>
+    </row>
+    <row r="666" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A666" s="4"/>
+    </row>
+    <row r="667" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A667" s="4"/>
+    </row>
+    <row r="668" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A668" s="4"/>
+    </row>
+    <row r="669" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A669" s="4"/>
+    </row>
+    <row r="670" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A670" s="4"/>
+    </row>
+    <row r="671" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A671" s="4"/>
+    </row>
+    <row r="672" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A672" s="4"/>
+    </row>
+    <row r="673" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A673" s="4"/>
+    </row>
+    <row r="674" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A674" s="4"/>
+    </row>
+    <row r="675" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A675" s="4"/>
+    </row>
+    <row r="676" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A676" s="4"/>
+    </row>
+    <row r="677" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A677" s="4"/>
+    </row>
+    <row r="678" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A678" s="4"/>
+    </row>
+    <row r="679" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A679" s="4"/>
+    </row>
+    <row r="680" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A680" s="4"/>
+    </row>
+    <row r="681" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A681" s="4"/>
+    </row>
+    <row r="682" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A682" s="4"/>
+    </row>
+    <row r="683" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A683" s="4"/>
+    </row>
+    <row r="684" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A684" s="4"/>
+    </row>
+    <row r="685" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A685" s="4"/>
+    </row>
+    <row r="686" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A686" s="4"/>
+    </row>
+    <row r="687" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A687" s="4"/>
+    </row>
+    <row r="688" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A688" s="4"/>
+    </row>
+    <row r="689" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A689" s="4"/>
+    </row>
+    <row r="690" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A690" s="4"/>
+    </row>
+    <row r="691" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A691" s="4"/>
+    </row>
+    <row r="692" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A692" s="4"/>
+    </row>
+    <row r="693" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A693" s="4"/>
+    </row>
+    <row r="694" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A694" s="4"/>
+    </row>
+    <row r="695" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A695" s="4"/>
+    </row>
+    <row r="696" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A696" s="4"/>
+    </row>
+    <row r="697" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A697" s="4"/>
+    </row>
+    <row r="698" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A698" s="4"/>
+    </row>
+    <row r="699" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A699" s="4"/>
+    </row>
+    <row r="700" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A700" s="4"/>
+    </row>
+    <row r="701" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A701" s="4"/>
+    </row>
+    <row r="702" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A702" s="4"/>
+    </row>
+    <row r="703" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A703" s="4"/>
+    </row>
+    <row r="704" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A704" s="4"/>
+    </row>
+    <row r="705" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A705" s="4"/>
+    </row>
+    <row r="706" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A706" s="4"/>
+    </row>
+    <row r="707" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A707" s="4"/>
+    </row>
+    <row r="708" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A708" s="4"/>
+    </row>
+    <row r="709" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A709" s="4"/>
+    </row>
+    <row r="710" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A710" s="4"/>
+    </row>
+    <row r="711" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A711" s="4"/>
+    </row>
+    <row r="712" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A712" s="4"/>
+    </row>
+    <row r="713" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A713" s="4"/>
+    </row>
+    <row r="714" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A714" s="4"/>
+    </row>
+    <row r="715" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A715" s="4"/>
+    </row>
+    <row r="716" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A716" s="4"/>
+    </row>
+    <row r="717" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A717" s="4"/>
+    </row>
+    <row r="718" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A718" s="4"/>
+    </row>
+    <row r="719" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A719" s="4"/>
+    </row>
+    <row r="720" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A720" s="4"/>
+    </row>
+    <row r="721" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A721" s="4"/>
+    </row>
+    <row r="722" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A722" s="4"/>
+    </row>
+    <row r="723" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A723" s="4"/>
+    </row>
+    <row r="724" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A724" s="4"/>
+    </row>
+    <row r="725" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A725" s="4"/>
+    </row>
+    <row r="726" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A726" s="4"/>
+    </row>
+    <row r="727" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A727" s="4"/>
+    </row>
+    <row r="728" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A728" s="4"/>
+    </row>
+    <row r="729" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A729" s="4"/>
+    </row>
+    <row r="730" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A730" s="4"/>
+    </row>
+    <row r="731" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A731" s="4"/>
+    </row>
+    <row r="732" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A732" s="4"/>
+    </row>
+    <row r="733" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A733" s="4"/>
+    </row>
+    <row r="734" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A734" s="4"/>
+    </row>
+    <row r="735" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A735" s="4"/>
+    </row>
+    <row r="736" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A736" s="4"/>
+    </row>
+    <row r="737" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A737" s="4"/>
+    </row>
+    <row r="738" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A738" s="4"/>
+    </row>
+    <row r="739" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A739" s="4"/>
+    </row>
+    <row r="740" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A740" s="4"/>
+    </row>
+    <row r="741" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A741" s="4"/>
+    </row>
+    <row r="742" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A742" s="4"/>
+    </row>
+    <row r="743" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A743" s="4"/>
+    </row>
+    <row r="744" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A744" s="4"/>
+    </row>
+    <row r="745" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A745" s="4"/>
+    </row>
+    <row r="746" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A746" s="4"/>
+    </row>
+    <row r="747" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A747" s="4"/>
+    </row>
+    <row r="748" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A748" s="4"/>
+    </row>
+    <row r="749" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A749" s="4"/>
+    </row>
+    <row r="750" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A750" s="4"/>
+    </row>
+    <row r="751" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A751" s="4"/>
+    </row>
+    <row r="752" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A752" s="4"/>
+    </row>
+    <row r="753" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A753" s="4"/>
+    </row>
+    <row r="754" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A754" s="4"/>
+    </row>
+    <row r="755" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A755" s="4"/>
+    </row>
+    <row r="756" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A756" s="4"/>
+    </row>
+    <row r="757" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A757" s="4"/>
+    </row>
+    <row r="758" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A758" s="4"/>
+    </row>
+    <row r="759" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A759" s="4"/>
+    </row>
+    <row r="760" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A760" s="4"/>
+    </row>
+    <row r="761" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A761" s="4"/>
+    </row>
+    <row r="762" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A762" s="4"/>
+    </row>
+    <row r="763" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A763" s="4"/>
+    </row>
+    <row r="764" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A764" s="4"/>
+    </row>
+    <row r="765" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A765" s="4"/>
+    </row>
+    <row r="766" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A766" s="4"/>
+    </row>
+    <row r="767" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A767" s="4"/>
+    </row>
+    <row r="768" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A768" s="4"/>
+    </row>
+    <row r="769" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A769" s="4"/>
+    </row>
+    <row r="770" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A770" s="4"/>
+    </row>
+    <row r="771" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A771" s="4"/>
+    </row>
+    <row r="772" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A772" s="4"/>
+    </row>
+    <row r="773" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A773" s="4"/>
+    </row>
+    <row r="774" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A774" s="4"/>
+    </row>
+    <row r="775" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A775" s="4"/>
+    </row>
+    <row r="776" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A776" s="4"/>
+    </row>
+    <row r="777" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A777" s="4"/>
+    </row>
+    <row r="778" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A778" s="4"/>
+    </row>
+    <row r="779" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A779" s="4"/>
+    </row>
+    <row r="780" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A780" s="4"/>
+    </row>
+    <row r="781" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A781" s="4"/>
+    </row>
+    <row r="782" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A782" s="4"/>
+    </row>
+    <row r="783" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A783" s="4"/>
+    </row>
+    <row r="784" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A784" s="4"/>
+    </row>
+    <row r="785" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A785" s="4"/>
+    </row>
+    <row r="786" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A786" s="4"/>
+    </row>
+    <row r="787" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A787" s="4"/>
+    </row>
+    <row r="788" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A788" s="4"/>
+    </row>
+    <row r="789" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A789" s="4"/>
+    </row>
+    <row r="790" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A790" s="4"/>
+    </row>
+    <row r="791" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A791" s="4"/>
+    </row>
+    <row r="792" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A792" s="4"/>
+    </row>
+    <row r="793" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A793" s="4"/>
+    </row>
+    <row r="794" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A794" s="4"/>
+    </row>
+    <row r="795" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A795" s="4"/>
+    </row>
+    <row r="796" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A796" s="4"/>
+    </row>
+    <row r="797" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A797" s="4"/>
+    </row>
+    <row r="798" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A798" s="4"/>
+    </row>
+    <row r="799" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A799" s="4"/>
+    </row>
+    <row r="800" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A800" s="4"/>
+    </row>
+    <row r="801" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A801" s="4"/>
+    </row>
+    <row r="802" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A802" s="4"/>
+    </row>
+    <row r="803" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A803" s="4"/>
+    </row>
+    <row r="804" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A804" s="4"/>
+    </row>
+    <row r="805" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A805" s="4"/>
+    </row>
+    <row r="806" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A806" s="4"/>
+    </row>
+    <row r="807" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A807" s="4"/>
+    </row>
+    <row r="808" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A808" s="4"/>
+    </row>
+    <row r="809" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A809" s="4"/>
+    </row>
+    <row r="810" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A810" s="4"/>
+    </row>
+    <row r="811" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A811" s="4"/>
+    </row>
+    <row r="812" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A812" s="4"/>
+    </row>
+    <row r="813" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A813" s="4"/>
+    </row>
+    <row r="814" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A814" s="4"/>
+    </row>
+    <row r="815" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A815" s="4"/>
+    </row>
+    <row r="816" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A816" s="4"/>
+    </row>
+    <row r="817" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A817" s="4"/>
+    </row>
+    <row r="818" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A818" s="4"/>
+    </row>
+    <row r="819" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A819" s="4"/>
+    </row>
+    <row r="820" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A820" s="4"/>
+    </row>
+    <row r="821" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A821" s="4"/>
+    </row>
+    <row r="822" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A822" s="4"/>
+    </row>
+    <row r="823" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A823" s="4"/>
+    </row>
+    <row r="824" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A824" s="4"/>
+    </row>
+    <row r="825" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A825" s="4"/>
+    </row>
+    <row r="826" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A826" s="4"/>
+    </row>
+    <row r="827" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A827" s="4"/>
+    </row>
+    <row r="828" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A828" s="4"/>
+    </row>
+    <row r="829" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A829" s="4"/>
+    </row>
+    <row r="830" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A830" s="4"/>
+    </row>
+    <row r="831" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A831" s="4"/>
+    </row>
+    <row r="832" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A832" s="4"/>
+    </row>
+    <row r="833" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A833" s="4"/>
+    </row>
+    <row r="834" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A834" s="4"/>
+    </row>
+    <row r="835" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A835" s="4"/>
+    </row>
+    <row r="836" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A836" s="4"/>
+    </row>
+    <row r="837" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A837" s="4"/>
+    </row>
+    <row r="838" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A838" s="4"/>
+    </row>
+    <row r="839" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A839" s="4"/>
+    </row>
+    <row r="840" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A840" s="4"/>
+    </row>
+    <row r="841" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A841" s="4"/>
+    </row>
+    <row r="842" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A842" s="4"/>
+    </row>
+    <row r="843" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A843" s="4"/>
+    </row>
+    <row r="844" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A844" s="4"/>
+    </row>
+    <row r="845" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A845" s="4"/>
+    </row>
+    <row r="846" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A846" s="4"/>
+    </row>
+    <row r="847" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A847" s="4"/>
+    </row>
+    <row r="848" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A848" s="4"/>
+    </row>
+    <row r="849" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A849" s="4"/>
+    </row>
+    <row r="850" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A850" s="4"/>
+    </row>
+    <row r="851" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A851" s="4"/>
+    </row>
+    <row r="852" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A852" s="4"/>
+    </row>
+    <row r="853" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A853" s="4"/>
+    </row>
+    <row r="854" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A854" s="4"/>
+    </row>
+    <row r="855" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A855" s="4"/>
+    </row>
+    <row r="856" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A856" s="4"/>
+    </row>
+    <row r="857" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A857" s="4"/>
+    </row>
+    <row r="858" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A858" s="4"/>
+    </row>
+    <row r="859" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A859" s="4"/>
+    </row>
+    <row r="860" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A860" s="4"/>
+    </row>
+    <row r="861" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A861" s="4"/>
+    </row>
+    <row r="862" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A862" s="4"/>
+    </row>
+    <row r="863" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A863" s="4"/>
+    </row>
+    <row r="864" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A864" s="4"/>
+    </row>
+    <row r="865" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A865" s="4"/>
+    </row>
+    <row r="866" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A866" s="4"/>
+    </row>
+    <row r="867" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A867" s="4"/>
+    </row>
+    <row r="868" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A868" s="4"/>
+    </row>
+    <row r="869" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A869" s="4"/>
+    </row>
+    <row r="870" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A870" s="4"/>
+    </row>
+    <row r="871" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A871" s="4"/>
+    </row>
+    <row r="872" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A872" s="4"/>
+    </row>
+    <row r="873" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A873" s="4"/>
+    </row>
+    <row r="874" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A874" s="4"/>
+    </row>
+    <row r="875" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A875" s="4"/>
+    </row>
+    <row r="876" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A876" s="4"/>
+    </row>
+    <row r="877" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A877" s="4"/>
+    </row>
+    <row r="878" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A878" s="4"/>
+    </row>
+    <row r="879" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A879" s="4"/>
+    </row>
+    <row r="880" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A880" s="4"/>
+    </row>
+    <row r="881" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A881" s="4"/>
+    </row>
+    <row r="882" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A882" s="4"/>
+    </row>
+    <row r="883" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A883" s="4"/>
+    </row>
+    <row r="884" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A884" s="4"/>
+    </row>
+    <row r="885" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A885" s="4"/>
+    </row>
+    <row r="886" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A886" s="4"/>
+    </row>
+    <row r="887" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A887" s="4"/>
+    </row>
+    <row r="888" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A888" s="4"/>
+    </row>
+    <row r="889" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A889" s="4"/>
+    </row>
+    <row r="890" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A890" s="4"/>
+    </row>
+    <row r="891" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A891" s="4"/>
+    </row>
+    <row r="892" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A892" s="4"/>
+    </row>
+    <row r="893" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A893" s="4"/>
+    </row>
+    <row r="894" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A894" s="4"/>
+    </row>
+    <row r="895" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A895" s="4"/>
+    </row>
+    <row r="896" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A896" s="4"/>
+    </row>
+    <row r="897" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A897" s="4"/>
+    </row>
+    <row r="898" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A898" s="4"/>
+    </row>
+    <row r="899" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A899" s="4"/>
+    </row>
+    <row r="900" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A900" s="4"/>
+    </row>
+    <row r="901" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A901" s="4"/>
+    </row>
+    <row r="902" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A902" s="4"/>
+    </row>
+    <row r="903" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A903" s="4"/>
+    </row>
+    <row r="904" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A904" s="4"/>
+    </row>
+    <row r="905" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A905" s="4"/>
+    </row>
+    <row r="906" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A906" s="4"/>
+    </row>
+    <row r="907" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A907" s="4"/>
+    </row>
+    <row r="908" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A908" s="4"/>
+    </row>
+    <row r="909" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A909" s="4"/>
+    </row>
+    <row r="910" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A910" s="4"/>
+    </row>
+    <row r="911" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A911" s="4"/>
+    </row>
+    <row r="912" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A912" s="4"/>
+    </row>
+    <row r="913" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A913" s="4"/>
+    </row>
+    <row r="914" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A914" s="4"/>
+    </row>
+    <row r="915" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A915" s="4"/>
+    </row>
+    <row r="916" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A916" s="4"/>
+    </row>
+    <row r="917" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A917" s="4"/>
+    </row>
+    <row r="918" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A918" s="4"/>
+    </row>
+    <row r="919" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A919" s="4"/>
+    </row>
+    <row r="920" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A920" s="4"/>
+    </row>
+    <row r="921" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A921" s="4"/>
+    </row>
+    <row r="922" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A922" s="4"/>
+    </row>
+    <row r="923" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A923" s="4"/>
+    </row>
+    <row r="924" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A924" s="4"/>
+    </row>
+    <row r="925" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A925" s="4"/>
+    </row>
+    <row r="926" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A926" s="4"/>
+    </row>
+    <row r="927" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A927" s="4"/>
+    </row>
+    <row r="928" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A928" s="4"/>
+    </row>
+    <row r="929" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A929" s="4"/>
+    </row>
+    <row r="930" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A930" s="4"/>
+    </row>
+    <row r="931" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A931" s="4"/>
+    </row>
+    <row r="932" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A932" s="4"/>
+    </row>
+    <row r="933" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A933" s="4"/>
+    </row>
+    <row r="934" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A934" s="4"/>
+    </row>
+    <row r="935" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A935" s="4"/>
+    </row>
+    <row r="936" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A936" s="4"/>
+    </row>
+    <row r="937" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A937" s="4"/>
+    </row>
+    <row r="938" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A938" s="4"/>
+    </row>
+    <row r="939" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A939" s="4"/>
+    </row>
+    <row r="940" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A940" s="4"/>
+    </row>
+    <row r="941" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A941" s="4"/>
+    </row>
+    <row r="942" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A942" s="4"/>
+    </row>
+    <row r="943" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A943" s="4"/>
+    </row>
+    <row r="944" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A944" s="4"/>
+    </row>
+    <row r="945" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A945" s="4"/>
+    </row>
+    <row r="946" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A946" s="4"/>
+    </row>
+    <row r="947" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A947" s="4"/>
+    </row>
+    <row r="948" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A948" s="4"/>
+    </row>
+    <row r="949" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A949" s="4"/>
+    </row>
+    <row r="950" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A950" s="4"/>
+    </row>
+    <row r="951" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A951" s="4"/>
+    </row>
+    <row r="952" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A952" s="4"/>
+    </row>
+    <row r="953" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A953" s="4"/>
+    </row>
+    <row r="954" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A954" s="4"/>
+    </row>
+    <row r="955" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A955" s="4"/>
+    </row>
+    <row r="956" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A956" s="4"/>
+    </row>
+    <row r="957" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A957" s="4"/>
+    </row>
+    <row r="958" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A958" s="4"/>
+    </row>
+    <row r="959" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A959" s="4"/>
+    </row>
+    <row r="960" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A960" s="4"/>
+    </row>
+    <row r="961" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A961" s="4"/>
+    </row>
+    <row r="962" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A962" s="4"/>
+    </row>
+    <row r="963" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A963" s="4"/>
+    </row>
+    <row r="964" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A964" s="4"/>
+    </row>
+    <row r="965" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A965" s="4"/>
+    </row>
+    <row r="966" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A966" s="4"/>
+    </row>
+    <row r="967" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A967" s="4"/>
+    </row>
+    <row r="968" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A968" s="4"/>
+    </row>
+    <row r="969" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A969" s="4"/>
+    </row>
+    <row r="970" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A970" s="4"/>
+    </row>
+    <row r="971" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A971" s="4"/>
+    </row>
+    <row r="972" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A972" s="4"/>
+    </row>
+    <row r="973" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A973" s="4"/>
+    </row>
+    <row r="974" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A974" s="4"/>
+    </row>
+    <row r="975" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A975" s="4"/>
+    </row>
+    <row r="976" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A976" s="4"/>
+    </row>
+    <row r="977" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A977" s="4"/>
+    </row>
+    <row r="978" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A978" s="4"/>
+    </row>
+    <row r="979" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A979" s="4"/>
+    </row>
+    <row r="980" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A980" s="4"/>
+    </row>
+    <row r="981" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A981" s="4"/>
+    </row>
+    <row r="982" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A982" s="4"/>
+    </row>
+    <row r="983" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A983" s="4"/>
+    </row>
+    <row r="984" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A984" s="4"/>
+    </row>
+    <row r="985" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A985" s="4"/>
+    </row>
+    <row r="986" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A986" s="4"/>
+    </row>
+    <row r="987" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A987" s="4"/>
+    </row>
+    <row r="988" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A988" s="4"/>
+    </row>
+    <row r="989" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A989" s="4"/>
+    </row>
+    <row r="990" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A990" s="4"/>
+    </row>
+    <row r="991" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A991" s="4"/>
+    </row>
+    <row r="992" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A992" s="4"/>
+    </row>
+    <row r="993" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A993" s="4"/>
+    </row>
+    <row r="994" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A994" s="4"/>
+    </row>
+    <row r="995" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A995" s="4"/>
+    </row>
+    <row r="996" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A996" s="4"/>
+    </row>
+    <row r="997" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A997" s="4"/>
+    </row>
+    <row r="998" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A998" s="4"/>
+    </row>
+    <row r="999" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A999" s="4"/>
+    </row>
+    <row r="1000" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A1000" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{9D539EDE-EB30-45F2-B81F-5A6E8575F40E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Break down the MMULT approach
</commit_message>
<xml_diff>
--- a/CH-117 Add Index Column.xlsx
+++ b/CH-117 Add Index Column.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C28B66-6301-4918-9611-B9CCE2AF10E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF0523F-D8C4-4E17-A3CB-E6456B23591E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,8 +94,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="0;\-0;0;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -327,7 +328,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -368,6 +369,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11012,10 +11014,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6670CB79-F1D1-4D4D-9198-51C23E9A3D45}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="E47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -11412,10 +11414,10 @@
     <row r="16" spans="1:26" ht="14.4" customHeight="1">
       <c r="A16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="14.4">
+    <row r="17" spans="1:17" ht="14.4">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="14.4" customHeight="1">
+    <row r="18" spans="1:17" ht="14.4" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="12" t="str" cm="1">
         <f t="array" ref="B18:D28">_xlfn.LET(_xlpm.b, B3:B13, _xlpm.r, ROW(_xlpm.b), _xlfn.HSTACK(B3:C13, MMULT((_xlpm.b=_xlfn.TOROW(_xlpm.b))*(_xlpm.r&gt;=_xlfn.TOROW(_xlpm.r)), _xlpm.r^0)))</f>
@@ -11427,8 +11429,42 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G18" t="str" cm="1">
+        <f t="array" ref="G18:Q18">_xlfn.TOROW(B3:B13)</f>
+        <v>A</v>
+      </c>
+      <c r="H18" t="str">
+        <v>A</v>
+      </c>
+      <c r="I18" t="str">
+        <v>A</v>
+      </c>
+      <c r="J18" t="str">
+        <v>B</v>
+      </c>
+      <c r="K18" t="str">
+        <v>B</v>
+      </c>
+      <c r="L18" t="str">
+        <v>A</v>
+      </c>
+      <c r="M18" t="str">
+        <v>B</v>
+      </c>
+      <c r="N18" t="str">
+        <v>A</v>
+      </c>
+      <c r="O18" t="str">
+        <v>A</v>
+      </c>
+      <c r="P18" t="str">
+        <v>B</v>
+      </c>
+      <c r="Q18" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="14.4" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" t="str">
         <v>A</v>
@@ -11440,7 +11476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.4" customHeight="1">
+    <row r="20" spans="1:17" ht="14.4" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" t="str">
         <v>A</v>
@@ -11451,8 +11487,42 @@
       <c r="D20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G20" t="b" cm="1">
+        <f t="array" ref="G20:Q30">(B3:B13=_xlfn.ANCHORARRAY(G18))</f>
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="14.4" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" t="str">
         <v>B</v>
@@ -11463,8 +11533,41 @@
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" t="b">
+        <v>1</v>
+      </c>
+      <c r="O21" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="14.4" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" t="str">
         <v>B</v>
@@ -11475,8 +11578,41 @@
       <c r="D22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O22" t="b">
+        <v>1</v>
+      </c>
+      <c r="P22" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="14.4" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" t="str">
         <v>A</v>
@@ -11487,8 +11623,41 @@
       <c r="D23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="14.4" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" t="str">
         <v>B</v>
@@ -11499,8 +11668,41 @@
       <c r="D24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="14.4" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" t="str">
         <v>A</v>
@@ -11511,8 +11713,41 @@
       <c r="D25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" t="b">
+        <v>1</v>
+      </c>
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="14.4" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" t="str">
         <v>A</v>
@@ -11523,8 +11758,41 @@
       <c r="D26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="14.4" customHeight="1">
       <c r="A27" s="4"/>
       <c r="B27" t="str">
         <v>B</v>
@@ -11535,8 +11803,41 @@
       <c r="D27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="14.4" customHeight="1">
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="14.4" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" t="str">
         <v>B</v>
@@ -11547,162 +11848,1091 @@
       <c r="D28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" customHeight="1">
       <c r="A29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" t="b">
+        <v>0</v>
+      </c>
+      <c r="P29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1">
       <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+    <row r="32" spans="1:17" ht="15.75" customHeight="1">
       <c r="A32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G32" t="b" cm="1">
+        <f t="array" ref="G32:Q42">ROW(B3:B13)&gt;=_xlfn.TOROW(ROW(B3:B13))</f>
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" customHeight="1">
       <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
+      </c>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33" t="b">
+        <v>0</v>
+      </c>
+      <c r="O33" t="b">
+        <v>0</v>
+      </c>
+      <c r="P33" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15.75" customHeight="1">
       <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+      <c r="N34" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" t="b">
+        <v>0</v>
+      </c>
+      <c r="P34" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" customHeight="1">
       <c r="A35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+      <c r="D35" s="1"/>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+      <c r="N35" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35" t="b">
+        <v>0</v>
+      </c>
+      <c r="P35" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" customHeight="1">
       <c r="A36" s="4"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
+      </c>
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" t="b">
+        <v>0</v>
+      </c>
+      <c r="P36" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1">
       <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37" t="b">
+        <v>0</v>
+      </c>
+      <c r="O37" t="b">
+        <v>0</v>
+      </c>
+      <c r="P37" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1">
       <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" t="b">
+        <v>0</v>
+      </c>
+      <c r="P38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1">
       <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
+      <c r="M39" t="b">
+        <v>1</v>
+      </c>
+      <c r="N39" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" t="b">
+        <v>0</v>
+      </c>
+      <c r="P39" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1">
       <c r="A40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="b">
+        <v>1</v>
+      </c>
+      <c r="M40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40" t="b">
+        <v>1</v>
+      </c>
+      <c r="O40" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15.75" customHeight="1">
       <c r="A41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
+      <c r="N41" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="15.75" customHeight="1">
       <c r="A42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
+      <c r="M42" t="b">
+        <v>1</v>
+      </c>
+      <c r="N42" t="b">
+        <v>1</v>
+      </c>
+      <c r="O42" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="15.75" customHeight="1">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+    <row r="44" spans="1:17" ht="15.75" customHeight="1">
       <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G44" cm="1">
+        <f t="array" ref="G44:Q54">_xlfn.ANCHORARRAY(G20)*_xlfn.ANCHORARRAY(G32)</f>
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="15.75" customHeight="1">
       <c r="A45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15.75" customHeight="1">
       <c r="A46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="15.75" customHeight="1">
       <c r="A47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="15.75" customHeight="1">
       <c r="A48" s="4"/>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="15.75" customHeight="1">
       <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="15.75" customHeight="1">
       <c r="A50" s="4"/>
-    </row>
-    <row r="51" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1">
       <c r="A51" s="4"/>
-    </row>
-    <row r="52" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1">
       <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1">
       <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="15.75" customHeight="1">
       <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="15.75" customHeight="1">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:1" ht="15.75" customHeight="1">
+    <row r="56" spans="1:17" ht="15.75" customHeight="1">
       <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G56" s="16" cm="1">
+        <f t="array" ref="G56:G66">ROW(B3:B13)^0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="15.75" customHeight="1">
       <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G57" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="15.75" customHeight="1">
       <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G58" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="15.75" customHeight="1">
       <c r="A59" s="4"/>
-    </row>
-    <row r="60" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G59" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="15.75" customHeight="1">
       <c r="A60" s="4"/>
-    </row>
-    <row r="61" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G60" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1">
       <c r="A61" s="4"/>
-    </row>
-    <row r="62" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G61" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1">
       <c r="A62" s="4"/>
-    </row>
-    <row r="63" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G62" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1">
       <c r="A63" s="4"/>
-    </row>
-    <row r="64" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G63" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1">
       <c r="A64" s="4"/>
-    </row>
-    <row r="65" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G64" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" customHeight="1">
       <c r="A65" s="4"/>
-    </row>
-    <row r="66" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G65" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" customHeight="1">
       <c r="A66" s="4"/>
-    </row>
-    <row r="67" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G66" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" customHeight="1">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" spans="1:1" ht="15.75" customHeight="1">
+    <row r="68" spans="1:8" ht="15.75" customHeight="1">
       <c r="A68" s="4"/>
-    </row>
-    <row r="69" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G68" cm="1">
+        <f t="array" ref="G68:G78">MMULT(_xlfn.ANCHORARRAY(G44),_xlfn.ANCHORARRAY(G56))</f>
+        <v>1</v>
+      </c>
+      <c r="H68" t="b" cm="1">
+        <f t="array" ref="H68:H78">_xlfn.ANCHORARRAY(G68)=G3:G13</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" customHeight="1">
       <c r="A69" s="4"/>
-    </row>
-    <row r="70" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" customHeight="1">
       <c r="A70" s="4"/>
-    </row>
-    <row r="71" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" customHeight="1">
       <c r="A71" s="4"/>
-    </row>
-    <row r="72" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" customHeight="1">
       <c r="A72" s="4"/>
-    </row>
-    <row r="73" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" customHeight="1">
       <c r="A73" s="4"/>
-    </row>
-    <row r="74" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G73">
+        <v>4</v>
+      </c>
+      <c r="H73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" customHeight="1">
       <c r="A74" s="4"/>
-    </row>
-    <row r="75" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G74">
+        <v>3</v>
+      </c>
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" customHeight="1">
       <c r="A75" s="4"/>
-    </row>
-    <row r="76" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G75">
+        <v>5</v>
+      </c>
+      <c r="H75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" customHeight="1">
       <c r="A76" s="4"/>
-    </row>
-    <row r="77" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G76">
+        <v>6</v>
+      </c>
+      <c r="H76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" customHeight="1">
       <c r="A77" s="4"/>
-    </row>
-    <row r="78" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G77">
+        <v>4</v>
+      </c>
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" customHeight="1">
       <c r="A78" s="4"/>
-    </row>
-    <row r="79" spans="1:1" ht="15.75" customHeight="1">
+      <c r="G78">
+        <v>5</v>
+      </c>
+      <c r="H78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" customHeight="1">
       <c r="A79" s="4"/>
     </row>
-    <row r="80" spans="1:1" ht="15.75" customHeight="1">
+    <row r="80" spans="1:8" ht="15.75" customHeight="1">
       <c r="A80" s="4"/>
     </row>
     <row r="81" spans="1:1" ht="15.75" customHeight="1">
@@ -14461,9 +15691,6 @@
     </row>
     <row r="999" spans="1:1" ht="15.75" customHeight="1">
       <c r="A999" s="4"/>
-    </row>
-    <row r="1000" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A1000" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>